<commit_message>
replace total expenditure on education with separated private and public expenditure
</commit_message>
<xml_diff>
--- a/DataSources/Education expenditure/OECD_EducationExpenditure_level3-8_PublicPrivateSplit.xlsx
+++ b/DataSources/Education expenditure/OECD_EducationExpenditure_level3-8_PublicPrivateSplit.xlsx
@@ -5,17 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dystg\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dystg\OneDrive\my\research\matlab\ProjectSurrey\data\Education expenditure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C048849-3E14-496C-82DD-09D55385BFB8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{F19308A0-573D-44F3-9944-F63DFBD37441}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{02089891-E237-46BF-9D7B-137FFAA6D95A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11592" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OECD.Stat export" sheetId="1" r:id="rId1"/>
-    <sheet name="Private SUM" sheetId="4" r:id="rId2"/>
-    <sheet name="Public SUM" sheetId="3" r:id="rId3"/>
+    <sheet name="Private 3-8" sheetId="4" r:id="rId2"/>
+    <sheet name="Private Interp" sheetId="5" r:id="rId3"/>
+    <sheet name="Public 3-8" sheetId="3" r:id="rId4"/>
+    <sheet name="Public Interp" sheetId="6" r:id="rId5"/>
+    <sheet name="SUM of interp" sheetId="7" r:id="rId6"/>
+    <sheet name="interp of SUM" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -6904,7 +6908,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="59">
   <si>
     <t>&lt;?xml version="1.0" encoding="utf-16"?&gt;&lt;WebTableParameter xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns="http://stats.oecd.org/OECDStatWS/2004/03/01/"&gt;&lt;DataTable Code="EAG_FIN_RATIO_CATEGORY" HasMetadata="true"&gt;&lt;Name LocaleIsoCode="en"&gt;Educational finance indicators&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Indicateurs relatifs au financement de l’éducation&lt;/Name&gt;&lt;Dimension Code="COUNTRY" HasMetadata="false" CommonCode="LOCATION" Display="labels"&gt;&lt;Name LocaleIsoCode="en"&gt;Country&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Country&lt;/Name&gt;&lt;Member Code="AUS" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Australia&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Australie&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="BEL" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Belgium&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Belgique&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="CAN" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Canada&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Canada&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="DNK" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Denmark&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Danemark&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="FIN" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Finland&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Finlande&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="FRA" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;France&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;France&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="DEU" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Germany&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Allemagne&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="ITA" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Italy&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Italie&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="JPN" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Japan&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Japon&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="NLD" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Netherlands&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Pays-Bas&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="NOR" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Norway&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Norvège&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="PRT" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Portugal&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Portugal&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="ESP" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Spain&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Espagne&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="SWE" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Sweden&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Suède&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="CHE" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Switzerland&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Suisse&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="GBR" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;United Kingdom&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Royaume-Uni&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="USA" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;United States&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;États-Unis&lt;/Name&gt;&lt;/Member&gt;&lt;/Dimension&gt;&lt;Dimension Code="ISC11_LEVEL_CAT" HasMetadata="false" Display="labels"&gt;&lt;Name LocaleIsoCode="en"&gt;Education level and programe orientation&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Education level and programe orientation&lt;/Name&gt;&lt;Member Code="L5T8" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Total tertiary education (ISCED2011 levels 5 to 8)&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Ensemble de l’enseignement tertiaire (niveaux 5 à 8 de la CITE 2011)&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="L3T4" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Upper secondary and post-secondary non-tertiary education&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Upper secondary and post-secondary non-tertiary education&lt;/Name&gt;&lt;/Member&gt;&lt;/Dimension&gt;&lt;Dimension Code="INDICATOR" HasMetadata="false" Display="labels"&gt;&lt;Name LocaleIsoCode="en"&gt;Indicator&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Indicator&lt;/Name&gt;&lt;Member Code="FIN_GDP" HasMetadata="true" HasOnlyUnitMetadata="true" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Expenditure as a percentage of GDP&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Expenditure as a percentage of GDP&lt;/Name&gt;&lt;/Member&gt;&lt;/Dimension&gt;&lt;Dimension Code="EXPENDITURE_TYPE" HasMetadata="false" Display="labels"&gt;&lt;Name LocaleIsoCode="en"&gt;Type of expenditure&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Type of expenditure &lt;/Name&gt;&lt;Member Code="T" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;All expenditure types&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Tous types de dépenses confondus &lt;/Name&gt;&lt;/Member&gt;&lt;/Dimension&gt;&lt;Dimension Code="REF_SECTOR" HasMetadata="false" Display="labels"&gt;&lt;Name LocaleIsoCode="en"&gt;Source of funds&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Source de financement&lt;/Name&gt;&lt;Member Code="S13" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0" IsDisplayed="true"&gt;&lt;Name LocaleIsoCode="en"&gt;General government&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Exécutif général &lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="S1D" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Non-educational private sector&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Non-educational private sector&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="T" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Total&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Total&lt;/Name&gt;&lt;/Member&gt;&lt;/Dimension&gt;&lt;Dimension Code="COUNTERPART_SECTOR" HasMetadata="false" Display="labels"&gt;&lt;Name LocaleIsoCode="en"&gt;Institution type&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Type d'institution&lt;/Name&gt;&lt;Member Code="INST_T" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;All public and private educational institutions&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Ensemble des établissements d’enseignement publics et privés &lt;/Name&gt;&lt;/Member&gt;&lt;/Dimension&gt;&lt;Dimension Code="YEAR" HasMetadata="false" CommonCode="TIME" Display="labels"&gt;&lt;Name LocaleIsoCode="en"&gt;Year&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Year&lt;/Name&gt;&lt;Member Code="1995" HasMetadata="false"&gt;&lt;Name LocaleIsoCode="en"&gt;1995&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;1995&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="2000" HasMetadata="false"&gt;&lt;Name LocaleIsoCode="en"&gt;2000&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;2000&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="2005" HasMetadata="false"&gt;&lt;Name LocaleIsoCode="en"&gt;2005&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;2005&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="2008" HasMetadata="false"&gt;&lt;Name LocaleIsoCode="en"&gt;2008&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;2008&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="2009" HasMetadata="false"&gt;&lt;Name LocaleIsoCode="en"&gt;2009&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;2009&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="2010" HasMetadata="false"&gt;&lt;Name LocaleIsoCode="en"&gt;2010&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;2010&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="2011" HasMetadata="false"&gt;&lt;Name LocaleIsoCode="en"&gt;2011&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;2011&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="2012" HasMetadata="false"&gt;&lt;Name LocaleIsoCode="en"&gt;2012&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;2012&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="2013" HasMetadata="false"&gt;&lt;Name LocaleIsoCode="en"&gt;2013&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;2013&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="2014" HasMetadata="false"&gt;&lt;Name LocaleIsoCode="en"&gt;2014&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;2014&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="2015" HasMetadata="false"&gt;&lt;Name LocaleIsoCode="en"&gt;2015&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;2015&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="2016" HasMetadata="false"&gt;&lt;Name LocaleIsoCode="en"&gt;2016&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;2016&lt;/Name&gt;&lt;/Member&gt;&lt;/Dimension&gt;&lt;WBOSInformations&gt;&lt;TimeDimension WebTreeWasUsed="false"&gt;&lt;StartCodes Annual="1995" /&gt;&lt;EndCodes Annual="2016" /&gt;&lt;/TimeDimension&gt;&lt;/WBOSInformations&gt;&lt;Tabulation Axis="horizontal"&gt;&lt;Dimension Code="YEAR" CommonCode="TIME" /&gt;&lt;/Tabulation&gt;&lt;Tabulation Axis="vertical"&gt;&lt;Dimension Code="COUNTRY" CommonCode="LOCATION" /&gt;&lt;Dimension Code="ISC11_LEVEL_CAT" /&gt;&lt;Dimension Code="REF_SECTOR" /&gt;&lt;/Tabulation&gt;&lt;Tabulation Axis="page"&gt;&lt;Dimension Code="INDICATOR" /&gt;&lt;Dimension Code="EXPENDITURE_TYPE" /&gt;&lt;Dimension Code="COUNTERPART_SECTOR" /&gt;&lt;/Tabulation&gt;&lt;Formatting&gt;&lt;Labels LocaleIsoCode="en" /&gt;&lt;Power&gt;0&lt;/Power&gt;&lt;Decimals&gt;1&lt;/Decimals&gt;&lt;SkipEmptyLines&gt;true&lt;/SkipEmptyLines&gt;&lt;SkipEmptyCols&gt;false&lt;/SkipEmptyCols&gt;&lt;SkipLineHierarchy&gt;false&lt;/SkipLineHierarchy&gt;&lt;SkipColHierarchy&gt;false&lt;/SkipColHierarchy&gt;&lt;Page&gt;1&lt;/Page&gt;&lt;/Formatting&gt;&lt;/DataTable&gt;&lt;Format&gt;&lt;ShowEmptyAxes&gt;true&lt;/ShowEmptyAxes&gt;&lt;Page&gt;1&lt;/Page&gt;&lt;EnableSort&gt;true&lt;/EnableSort&gt;&lt;IncludeFlagColumn&gt;false&lt;/IncludeFlagColumn&gt;&lt;IncludeTimeSeriesId&gt;false&lt;/IncludeTimeSeriesId&gt;&lt;DoBarChart&gt;false&lt;/DoBarChart&gt;&lt;FreezePanes&gt;true&lt;/FreezePanes&gt;&lt;MaxBarChartLen&gt;65&lt;/MaxBarChartLen&gt;&lt;/Format&gt;&lt;Query&gt;&lt;AbsoluteUri&gt;http://stats.oecd.org//View.aspx?QueryId=77054&amp;amp;QueryType=Public&amp;amp;Lang=en&lt;/AbsoluteUri&gt;&lt;/Query&gt;&lt;/WebTableParameter&gt;</t>
   </si>
@@ -7072,6 +7076,15 @@
   </si>
   <si>
     <t>Not applicable</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Note: This is direct interpolation of the (pub+pri) level 3-8 spending. interpolating the components separately ought to behave better than interpolating the sum.</t>
   </si>
 </sst>
 </file>
@@ -8181,14 +8194,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P114"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="L96" sqref="L96"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="2.38671875" customWidth="1"/>
+    <col min="1" max="3" width="26.71875" customWidth="1"/>
+    <col min="4" max="4" width="2.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" hidden="1" x14ac:dyDescent="0.4">
@@ -13270,8 +13283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA69686-E91C-4338-B079-6B0A31053355}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -13648,11 +13661,624 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8346954-B4DC-4E7C-8279-3141F41D50AF}">
+  <dimension ref="A1:AG17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13:F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="8" max="12" width="9.1640625" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="8.88671875" customWidth="1"/>
+    <col min="22" max="29" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>2000</v>
+      </c>
+      <c r="B2">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="Q2">
+        <v>0.66100000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <f t="shared" ref="A4:A9" si="0">A3+1</f>
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>2005</v>
+      </c>
+      <c r="B7">
+        <v>1.012</v>
+      </c>
+      <c r="Q7">
+        <v>0.755</v>
+      </c>
+      <c r="AD7">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="AE7">
+        <v>0.52300000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>2008</v>
+      </c>
+      <c r="B10">
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="Q10">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="AD10">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="AE10">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>2009</v>
+      </c>
+      <c r="B11">
+        <v>1.0820000000000001</v>
+      </c>
+      <c r="Q11">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="AD11">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>2010</v>
+      </c>
+      <c r="B12">
+        <v>1.103</v>
+      </c>
+      <c r="Q12">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="AD12">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="AE12">
+        <v>0.52700000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>2011</v>
+      </c>
+      <c r="B13">
+        <v>1.091</v>
+      </c>
+      <c r="C13">
+        <v>1.244</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:E13" si="1">D14/EXP($L14)</f>
+        <v>1.095024773609224</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>5.9799920492535956E-2</v>
+      </c>
+      <c r="F13">
+        <f>F14/EXP($L14)</f>
+        <v>0.43232401536407145</v>
+      </c>
+      <c r="Q13">
+        <v>0.879</v>
+      </c>
+      <c r="AD13">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="AE13">
+        <v>0.505</v>
+      </c>
+      <c r="AG13">
+        <v>1.7929999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>2012</v>
+      </c>
+      <c r="B14">
+        <v>1.0880000000000001</v>
+      </c>
+      <c r="C14">
+        <v>1.298</v>
+      </c>
+      <c r="D14">
+        <v>1.117</v>
+      </c>
+      <c r="E14">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="F14">
+        <v>0.441</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14:H17" si="2">LN(B14)-LN(B13)</f>
+        <v>-2.7535584171827776E-3</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ref="I14:K17" si="3">LN(C14)-LN(C13)</f>
+        <v>4.2492623964910603E-2</v>
+      </c>
+      <c r="L14">
+        <f>AVERAGE(H14:I14)</f>
+        <v>1.9869532773863913E-2</v>
+      </c>
+      <c r="M14">
+        <v>0.214</v>
+      </c>
+      <c r="N14">
+        <f>N15/EXP(AC15)</f>
+        <v>0.10628244994566344</v>
+      </c>
+      <c r="O14">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="P14">
+        <v>0.37</v>
+      </c>
+      <c r="Q14">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="R14">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="S14">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="T14">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="AD14">
+        <v>0.437</v>
+      </c>
+      <c r="AE14">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="AF14">
+        <v>1.0189999999999999</v>
+      </c>
+      <c r="AG14">
+        <v>1.843</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>2013</v>
+      </c>
+      <c r="B15">
+        <v>1.18</v>
+      </c>
+      <c r="C15">
+        <v>1.3959999999999999</v>
+      </c>
+      <c r="D15">
+        <v>1.103</v>
+      </c>
+      <c r="E15">
+        <v>6.3E-2</v>
+      </c>
+      <c r="F15">
+        <f>F14*EXP(L15)</f>
+        <v>0.46056169242545109</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>8.1173290043822371E-2</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>7.278638605828236E-2</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>-1.261277981569825E-2</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="3"/>
+        <v>3.2260862218221664E-2</v>
+      </c>
+      <c r="L15">
+        <f t="shared" ref="L15:L16" si="4">AVERAGE(H15:K15)</f>
+        <v>4.3401939626157036E-2</v>
+      </c>
+      <c r="M15">
+        <v>0.222</v>
+      </c>
+      <c r="N15">
+        <v>0.105</v>
+      </c>
+      <c r="O15">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="P15">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="Q15">
+        <v>0.878</v>
+      </c>
+      <c r="R15">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="S15">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="T15">
+        <f>T14*EXP(AC15)</f>
+        <v>0.17190044084738804</v>
+      </c>
+      <c r="V15">
+        <f>LN(M15)-LN(M14)</f>
+        <v>3.670136685042813E-2</v>
+      </c>
+      <c r="X15">
+        <f t="shared" ref="X15:AB15" si="5">LN(O15)-LN(O14)</f>
+        <v>-2.2223136784710107E-2</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="5"/>
+        <v>-2.4625047305389169E-2</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="5"/>
+        <v>-1.9177124639738724E-2</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="5"/>
+        <v>-0.16812041020673005</v>
+      </c>
+      <c r="AB15">
+        <f t="shared" si="5"/>
+        <v>0.12460541845544426</v>
+      </c>
+      <c r="AC15">
+        <f t="shared" ref="AC15" si="6">AVERAGE(V15,X15:AB15)</f>
+        <v>-1.213982227178261E-2</v>
+      </c>
+      <c r="AD15">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="AE15">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="AF15">
+        <v>1.0660000000000001</v>
+      </c>
+      <c r="AG15">
+        <v>1.7869999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>2014</v>
+      </c>
+      <c r="B16">
+        <v>1.3460000000000001</v>
+      </c>
+      <c r="C16">
+        <v>1.417</v>
+      </c>
+      <c r="D16">
+        <v>1.109</v>
+      </c>
+      <c r="E16">
+        <v>6.2E-2</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ref="F16:F17" si="7">F15*EXP(L16)</f>
+        <v>0.47648746151761151</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>0.13162279274496277</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>1.493095636836278E-2</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>5.4249680968645742E-3</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="3"/>
+        <v>-1.6000341346441349E-2</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="4"/>
+        <v>3.3994593965937195E-2</v>
+      </c>
+      <c r="M16">
+        <v>0.245</v>
+      </c>
+      <c r="N16">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="O16">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="P16">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="Q16">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="R16">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="S16">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="T16">
+        <f t="shared" ref="T16:T17" si="8">T15*EXP(AC16)</f>
+        <v>0.16828165743258508</v>
+      </c>
+      <c r="V16">
+        <f t="shared" ref="V16:V17" si="9">LN(M16)-LN(M15)</f>
+        <v>9.858082867244744E-2</v>
+      </c>
+      <c r="W16">
+        <f t="shared" ref="W16" si="10">LN(N16)-LN(N15)</f>
+        <v>-0.16532398042538343</v>
+      </c>
+      <c r="X16">
+        <f t="shared" ref="X16:X17" si="11">LN(O16)-LN(O15)</f>
+        <v>-9.4187215059700957E-2</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" ref="Y16:Y17" si="12">LN(P16)-LN(P15)</f>
+        <v>0.14420826346592042</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" ref="Z16:Z17" si="13">LN(Q16)-LN(Q15)</f>
+        <v>-1.1454878974766491E-2</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" ref="AA16:AA17" si="14">LN(R16)-LN(R15)</f>
+        <v>-0.12701413839225739</v>
+      </c>
+      <c r="AB16">
+        <f t="shared" ref="AB16:AB17" si="15">LN(S16)-LN(S15)</f>
+        <v>6.2565376143051132E-3</v>
+      </c>
+      <c r="AC16">
+        <f>AVERAGE(V16:AB16)</f>
+        <v>-2.1276369014205043E-2</v>
+      </c>
+      <c r="AD16">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="AE16">
+        <v>0.505</v>
+      </c>
+      <c r="AF16">
+        <v>1.5</v>
+      </c>
+      <c r="AG16">
+        <v>1.8460000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>2015</v>
+      </c>
+      <c r="B17">
+        <v>1.466</v>
+      </c>
+      <c r="C17">
+        <v>1.377</v>
+      </c>
+      <c r="D17">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="E17">
+        <v>9.4E-2</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="7"/>
+        <v>0.53397694460618539</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>8.540037224192365E-2</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>-2.8634740962025618E-2</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>-1.7281012127177559E-2</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="3"/>
+        <v>0.4161603972249126</v>
+      </c>
+      <c r="L17">
+        <f>AVERAGE(H17:K17)</f>
+        <v>0.11391125409440828</v>
+      </c>
+      <c r="M17">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="N17">
+        <f>N16*EXP(AC17)</f>
+        <v>8.9548100344731721E-2</v>
+      </c>
+      <c r="O17">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="P17">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="Q17">
+        <v>0.871</v>
+      </c>
+      <c r="R17">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="S17">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="8"/>
+        <v>0.16931800838147076</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="9"/>
+        <v>0.10086061033497407</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="11"/>
+        <v>1.2270092591814219E-2</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="12"/>
+        <v>-5.4200456897679494E-2</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="13"/>
+        <v>3.4502621921526089E-3</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" si="14"/>
+        <v>-9.5782732384592173E-2</v>
+      </c>
+      <c r="AB17">
+        <f t="shared" si="15"/>
+        <v>7.0239495375801653E-2</v>
+      </c>
+      <c r="AC17">
+        <f>AVERAGE(V17,X17:AB17)</f>
+        <v>6.1395452020784795E-3</v>
+      </c>
+      <c r="AD17">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="AE17">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="AF17">
+        <v>1.581</v>
+      </c>
+      <c r="AG17">
+        <v>1.784</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -14065,4 +14691,2663 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16213876-B6D4-4A83-AEA1-4B8E942D53FC}">
+  <dimension ref="A1:AI17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="8" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="23" max="31" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>2000</v>
+      </c>
+      <c r="B2">
+        <v>1.4710000000000001</v>
+      </c>
+      <c r="F2">
+        <v>2.0459999999999998</v>
+      </c>
+      <c r="R2">
+        <v>1.571</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <f t="shared" ref="A4:A9" si="0">A3+1</f>
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>2005</v>
+      </c>
+      <c r="B7">
+        <v>1.4550000000000001</v>
+      </c>
+      <c r="F7">
+        <v>2.2989999999999999</v>
+      </c>
+      <c r="R7">
+        <v>1.744</v>
+      </c>
+      <c r="AF7">
+        <v>2.3079999999999998</v>
+      </c>
+      <c r="AG7">
+        <v>1.718</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>2008</v>
+      </c>
+      <c r="B10">
+        <v>1.379</v>
+      </c>
+      <c r="F10">
+        <v>1.96</v>
+      </c>
+      <c r="R10">
+        <v>1.75</v>
+      </c>
+      <c r="AF10">
+        <v>2.3420000000000001</v>
+      </c>
+      <c r="AG10">
+        <v>1.7290000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>2009</v>
+      </c>
+      <c r="B11">
+        <v>1.482</v>
+      </c>
+      <c r="F11">
+        <v>2.1349999999999998</v>
+      </c>
+      <c r="R11">
+        <v>1.925</v>
+      </c>
+      <c r="AF11">
+        <v>2.5019999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>2010</v>
+      </c>
+      <c r="B12">
+        <v>1.5620000000000001</v>
+      </c>
+      <c r="F12">
+        <v>2.1080000000000001</v>
+      </c>
+      <c r="R12">
+        <v>1.9590000000000001</v>
+      </c>
+      <c r="AF12">
+        <v>2.44</v>
+      </c>
+      <c r="AG12">
+        <v>1.913</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>2011</v>
+      </c>
+      <c r="B13">
+        <v>1.4930000000000001</v>
+      </c>
+      <c r="C13">
+        <v>2.6829999999999998</v>
+      </c>
+      <c r="D13">
+        <f>D14/EXP($M14)</f>
+        <v>1.2100792977868873</v>
+      </c>
+      <c r="E13">
+        <f>E14/EXP($M14)</f>
+        <v>3.0836193692554179</v>
+      </c>
+      <c r="F13">
+        <v>2.1179999999999999</v>
+      </c>
+      <c r="R13">
+        <v>1.9410000000000001</v>
+      </c>
+      <c r="AF13">
+        <v>2.3359999999999999</v>
+      </c>
+      <c r="AG13">
+        <v>1.8979999999999999</v>
+      </c>
+      <c r="AI13">
+        <v>2.0059999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>2012</v>
+      </c>
+      <c r="B14">
+        <v>1.4470000000000001</v>
+      </c>
+      <c r="C14">
+        <v>2.6269999999999998</v>
+      </c>
+      <c r="D14">
+        <v>1.1910000000000001</v>
+      </c>
+      <c r="E14">
+        <v>3.0350000000000001</v>
+      </c>
+      <c r="F14">
+        <v>2.1280000000000001</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14:H17" si="1">LN(B14)-LN(B13)</f>
+        <v>-3.1295070907706557E-2</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ref="I14:I17" si="2">LN(C14)-LN(C13)</f>
+        <v>-2.1093060740084213E-2</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14:L17" si="3">LN(F14)-LN(F13)</f>
+        <v>4.7103243001833661E-3</v>
+      </c>
+      <c r="M14">
+        <f>AVERAGE(H14:I14,L14)</f>
+        <v>-1.5892602449202469E-2</v>
+      </c>
+      <c r="N14">
+        <v>2.9870000000000001</v>
+      </c>
+      <c r="O14">
+        <v>2.673</v>
+      </c>
+      <c r="P14">
+        <v>3.2829999999999999</v>
+      </c>
+      <c r="Q14">
+        <v>1.722</v>
+      </c>
+      <c r="R14">
+        <v>1.962</v>
+      </c>
+      <c r="S14">
+        <v>1.6890000000000001</v>
+      </c>
+      <c r="T14">
+        <v>1.6930000000000001</v>
+      </c>
+      <c r="U14">
+        <v>2.6459999999999999</v>
+      </c>
+      <c r="AF14">
+        <v>2.2850000000000001</v>
+      </c>
+      <c r="AG14">
+        <v>1.871</v>
+      </c>
+      <c r="AH14">
+        <v>2.12</v>
+      </c>
+      <c r="AI14">
+        <v>1.956</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>2013</v>
+      </c>
+      <c r="B15">
+        <v>1.4159999999999999</v>
+      </c>
+      <c r="C15">
+        <v>2.5350000000000001</v>
+      </c>
+      <c r="D15">
+        <v>1.1759999999999999</v>
+      </c>
+      <c r="E15">
+        <v>3.109</v>
+      </c>
+      <c r="F15">
+        <v>2.125</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>-2.165645237781888E-2</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>-3.5648873660256264E-2</v>
+      </c>
+      <c r="J15">
+        <f t="shared" ref="J15:J17" si="4">LN(D15)-LN(D14)</f>
+        <v>-1.2674440896727979E-2</v>
+      </c>
+      <c r="K15">
+        <f t="shared" ref="K15:K17" si="5">LN(E15)-LN(E14)</f>
+        <v>2.4089706565155078E-2</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="3"/>
+        <v>-1.4107691030178504E-3</v>
+      </c>
+      <c r="M15">
+        <f>AVERAGE(H15:L15)</f>
+        <v>-9.4601658945331797E-3</v>
+      </c>
+      <c r="N15">
+        <v>3.0619999999999998</v>
+      </c>
+      <c r="O15">
+        <v>2.7370000000000001</v>
+      </c>
+      <c r="P15">
+        <v>3.2280000000000002</v>
+      </c>
+      <c r="Q15">
+        <v>1.7829999999999999</v>
+      </c>
+      <c r="R15">
+        <v>1.9770000000000001</v>
+      </c>
+      <c r="S15">
+        <v>1.788</v>
+      </c>
+      <c r="T15">
+        <v>1.6859999999999999</v>
+      </c>
+      <c r="U15">
+        <v>2.6160000000000001</v>
+      </c>
+      <c r="W15">
+        <f>LN(N15)-LN(N14)</f>
+        <v>2.4798758001519206E-2</v>
+      </c>
+      <c r="X15">
+        <f t="shared" ref="X15:AD15" si="6">LN(O15)-LN(O14)</f>
+        <v>2.3660992901760047E-2</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="6"/>
+        <v>-1.6894888111753215E-2</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="6"/>
+        <v>3.4810932875464329E-2</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="6"/>
+        <v>7.6161830453085333E-3</v>
+      </c>
+      <c r="AB15">
+        <f t="shared" si="6"/>
+        <v>5.6961038925659291E-2</v>
+      </c>
+      <c r="AC15">
+        <f t="shared" si="6"/>
+        <v>-4.1432435713346649E-3</v>
+      </c>
+      <c r="AD15">
+        <f t="shared" si="6"/>
+        <v>-1.1402632097811671E-2</v>
+      </c>
+      <c r="AE15">
+        <f>AVERAGE(W15:AD15)</f>
+        <v>1.4425892746101482E-2</v>
+      </c>
+      <c r="AF15">
+        <v>2.2789999999999999</v>
+      </c>
+      <c r="AG15">
+        <v>1.853</v>
+      </c>
+      <c r="AH15">
+        <v>2.2909999999999999</v>
+      </c>
+      <c r="AI15">
+        <v>1.8340000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>2014</v>
+      </c>
+      <c r="B16">
+        <v>1.3959999999999999</v>
+      </c>
+      <c r="C16">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="D16">
+        <v>1.1679999999999999</v>
+      </c>
+      <c r="E16">
+        <v>3.0819999999999999</v>
+      </c>
+      <c r="F16">
+        <v>2.1549999999999998</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>-1.4224990931347326E-2</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>-1.791092656653015E-2</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="4"/>
+        <v>-6.8259650703998698E-3</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="5"/>
+        <v>-8.722394178692694E-3</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="3"/>
+        <v>1.401892117933079E-2</v>
+      </c>
+      <c r="M16">
+        <f t="shared" ref="M16:M17" si="7">AVERAGE(H16:L16)</f>
+        <v>-6.7330711135278496E-3</v>
+      </c>
+      <c r="N16">
+        <v>3.032</v>
+      </c>
+      <c r="O16">
+        <v>2.9510000000000001</v>
+      </c>
+      <c r="P16">
+        <v>3.1709999999999998</v>
+      </c>
+      <c r="Q16">
+        <v>1.7010000000000001</v>
+      </c>
+      <c r="R16">
+        <v>1.9710000000000001</v>
+      </c>
+      <c r="S16">
+        <v>1.7190000000000001</v>
+      </c>
+      <c r="T16">
+        <v>1.6379999999999999</v>
+      </c>
+      <c r="U16">
+        <v>2.5619999999999998</v>
+      </c>
+      <c r="W16">
+        <f t="shared" ref="W16:W17" si="8">LN(N16)-LN(N15)</f>
+        <v>-9.8458294553667169E-3</v>
+      </c>
+      <c r="X16">
+        <f t="shared" ref="X16" si="9">LN(O16)-LN(O15)</f>
+        <v>7.5281665902260375E-2</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" ref="Y16:Y17" si="10">LN(P16)-LN(P15)</f>
+        <v>-1.7815754851492116E-2</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" ref="Z16:Z17" si="11">LN(Q16)-LN(Q15)</f>
+        <v>-4.7081025467278548E-2</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" ref="AA16:AA17" si="12">LN(R16)-LN(R15)</f>
+        <v>-3.0395160178967595E-3</v>
+      </c>
+      <c r="AB16">
+        <f t="shared" ref="AB16:AB17" si="13">LN(S16)-LN(S15)</f>
+        <v>-3.9354950350610096E-2</v>
+      </c>
+      <c r="AC16">
+        <f t="shared" ref="AC16:AC17" si="14">LN(T16)-LN(T15)</f>
+        <v>-2.8882874148786042E-2</v>
+      </c>
+      <c r="AD16">
+        <f t="shared" ref="AD16:AD17" si="15">LN(U16)-LN(U15)</f>
+        <v>-2.0858230120409882E-2</v>
+      </c>
+      <c r="AE16">
+        <f>AVERAGE(W16:AD16)</f>
+        <v>-1.1449564313697473E-2</v>
+      </c>
+      <c r="AF16">
+        <v>2.2770000000000001</v>
+      </c>
+      <c r="AG16">
+        <v>1.8580000000000001</v>
+      </c>
+      <c r="AH16">
+        <v>1.8280000000000001</v>
+      </c>
+      <c r="AI16">
+        <v>1.7869999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>2015</v>
+      </c>
+      <c r="B17">
+        <v>1.3939999999999999</v>
+      </c>
+      <c r="C17">
+        <v>2.504</v>
+      </c>
+      <c r="D17">
+        <v>1.115</v>
+      </c>
+      <c r="E17">
+        <v>3.1469999999999998</v>
+      </c>
+      <c r="F17">
+        <v>2.1459999999999999</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>-1.4336920018485633E-3</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>5.606742761235739E-3</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="4"/>
+        <v>-4.6438479493953175E-2</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="5"/>
+        <v>2.0870881184345658E-2</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="3"/>
+        <v>-4.1850793472042458E-3</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="7"/>
+        <v>-5.1159253794849178E-3</v>
+      </c>
+      <c r="N17">
+        <v>2.9710000000000001</v>
+      </c>
+      <c r="O17">
+        <f>O16*EXP(AE17)</f>
+        <v>2.8876294036063208</v>
+      </c>
+      <c r="P17">
+        <v>3.0110000000000001</v>
+      </c>
+      <c r="Q17">
+        <v>1.655</v>
+      </c>
+      <c r="R17">
+        <v>1.988</v>
+      </c>
+      <c r="S17">
+        <v>1.696</v>
+      </c>
+      <c r="T17">
+        <v>1.6379999999999999</v>
+      </c>
+      <c r="U17">
+        <v>2.4430000000000001</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="8"/>
+        <v>-2.0323871299654517E-2</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="10"/>
+        <v>-5.1774746056613363E-2</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="11"/>
+        <v>-2.7415304584698541E-2</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" si="12"/>
+        <v>8.5880800637991861E-3</v>
+      </c>
+      <c r="AB17">
+        <f t="shared" si="13"/>
+        <v>-1.3470189031001056E-2</v>
+      </c>
+      <c r="AC17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <f t="shared" si="15"/>
+        <v>-4.7561411198938974E-2</v>
+      </c>
+      <c r="AE17">
+        <f>AVERAGE(W17,Y17:AD17)</f>
+        <v>-2.1708206015301039E-2</v>
+      </c>
+      <c r="AF17">
+        <v>2.2639999999999998</v>
+      </c>
+      <c r="AG17">
+        <v>1.8240000000000001</v>
+      </c>
+      <c r="AH17">
+        <v>1.6319999999999999</v>
+      </c>
+      <c r="AI17">
+        <v>1.7749999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055CDB84-5CFA-493D-BDDE-64AC11FF6162}">
+  <dimension ref="A1:AG17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="8" max="12" width="9.1640625" hidden="1" customWidth="1"/>
+    <col min="22" max="29" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>2000</v>
+      </c>
+      <c r="B2">
+        <f>IF(OR('Private Interp'!B2="",'Public Interp'!B2=""),"",'Private Interp'!B2+'Public Interp'!B2)</f>
+        <v>2.403</v>
+      </c>
+      <c r="C2" t="str">
+        <f>IF(OR('Private Interp'!C2="",'Public Interp'!C2=""),"",'Private Interp'!C2+'Public Interp'!C2)</f>
+        <v/>
+      </c>
+      <c r="D2" t="str">
+        <f>IF(OR('Private Interp'!D2="",'Public Interp'!D2=""),"",'Private Interp'!D2+'Public Interp'!D2)</f>
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(OR('Private Interp'!E2="",'Public Interp'!E2=""),"",'Private Interp'!E2+'Public Interp'!E2)</f>
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <f>IF(OR('Private Interp'!F2="",'Public Interp'!F2=""),"",'Private Interp'!F2+'Public Interp'!F2)</f>
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <f>IF(OR('Private Interp'!G2="",'Public Interp'!G2=""),"",'Private Interp'!G2+'Public Interp'!G2)</f>
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <f>IF(OR('Private Interp'!H2="",'Public Interp'!H2=""),"",'Private Interp'!H2+'Public Interp'!H2)</f>
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <f>IF(OR('Private Interp'!I2="",'Public Interp'!I2=""),"",'Private Interp'!I2+'Public Interp'!I2)</f>
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <f>IF(OR('Private Interp'!J2="",'Public Interp'!J2=""),"",'Private Interp'!J2+'Public Interp'!J2)</f>
+        <v/>
+      </c>
+      <c r="K2" t="str">
+        <f>IF(OR('Private Interp'!K2="",'Public Interp'!K2=""),"",'Private Interp'!K2+'Public Interp'!K2)</f>
+        <v/>
+      </c>
+      <c r="L2" t="str">
+        <f>IF(OR('Private Interp'!L2="",'Public Interp'!L2=""),"",'Private Interp'!L2+'Public Interp'!L2)</f>
+        <v/>
+      </c>
+      <c r="M2" t="str">
+        <f>IF(OR('Private Interp'!M2="",'Public Interp'!M2=""),"",'Private Interp'!M2+'Public Interp'!M2)</f>
+        <v/>
+      </c>
+      <c r="N2" t="str">
+        <f>IF(OR('Private Interp'!N2="",'Public Interp'!N2=""),"",'Private Interp'!N2+'Public Interp'!N2)</f>
+        <v/>
+      </c>
+      <c r="O2" t="str">
+        <f>IF(OR('Private Interp'!O2="",'Public Interp'!O2=""),"",'Private Interp'!O2+'Public Interp'!O2)</f>
+        <v/>
+      </c>
+      <c r="P2" t="str">
+        <f>IF(OR('Private Interp'!P2="",'Public Interp'!P2=""),"",'Private Interp'!P2+'Public Interp'!P2)</f>
+        <v/>
+      </c>
+      <c r="Q2" t="str">
+        <f>IF(OR('Private Interp'!Q2="",'Public Interp'!Q2=""),"",'Private Interp'!Q2+'Public Interp'!Q2)</f>
+        <v/>
+      </c>
+      <c r="R2" t="str">
+        <f>IF(OR('Private Interp'!R2="",'Public Interp'!R2=""),"",'Private Interp'!R2+'Public Interp'!R2)</f>
+        <v/>
+      </c>
+      <c r="S2" t="str">
+        <f>IF(OR('Private Interp'!S2="",'Public Interp'!S2=""),"",'Private Interp'!S2+'Public Interp'!S2)</f>
+        <v/>
+      </c>
+      <c r="T2" t="str">
+        <f>IF(OR('Private Interp'!T2="",'Public Interp'!T2=""),"",'Private Interp'!T2+'Public Interp'!T2)</f>
+        <v/>
+      </c>
+      <c r="U2" t="str">
+        <f>IF(OR('Private Interp'!U2="",'Public Interp'!U2=""),"",'Private Interp'!U2+'Public Interp'!U2)</f>
+        <v/>
+      </c>
+      <c r="V2" t="str">
+        <f>IF(OR('Private Interp'!V2="",'Public Interp'!V2=""),"",'Private Interp'!V2+'Public Interp'!V2)</f>
+        <v/>
+      </c>
+      <c r="W2" t="str">
+        <f>IF(OR('Private Interp'!W2="",'Public Interp'!W2=""),"",'Private Interp'!W2+'Public Interp'!W2)</f>
+        <v/>
+      </c>
+      <c r="X2" t="str">
+        <f>IF(OR('Private Interp'!X2="",'Public Interp'!X2=""),"",'Private Interp'!X2+'Public Interp'!X2)</f>
+        <v/>
+      </c>
+      <c r="Y2" t="str">
+        <f>IF(OR('Private Interp'!Y2="",'Public Interp'!Y2=""),"",'Private Interp'!Y2+'Public Interp'!Y2)</f>
+        <v/>
+      </c>
+      <c r="Z2" t="str">
+        <f>IF(OR('Private Interp'!Z2="",'Public Interp'!Z2=""),"",'Private Interp'!Z2+'Public Interp'!Z2)</f>
+        <v/>
+      </c>
+      <c r="AA2" t="str">
+        <f>IF(OR('Private Interp'!AA2="",'Public Interp'!AA2=""),"",'Private Interp'!AA2+'Public Interp'!AA2)</f>
+        <v/>
+      </c>
+      <c r="AB2" t="str">
+        <f>IF(OR('Private Interp'!AB2="",'Public Interp'!AB2=""),"",'Private Interp'!AB2+'Public Interp'!AB2)</f>
+        <v/>
+      </c>
+      <c r="AC2" t="str">
+        <f>IF(OR('Private Interp'!AC2="",'Public Interp'!AC2=""),"",'Private Interp'!AC2+'Public Interp'!AC2)</f>
+        <v/>
+      </c>
+      <c r="AD2" t="str">
+        <f>IF(OR('Private Interp'!AD2="",'Public Interp'!AD2=""),"",'Private Interp'!AD2+'Public Interp'!AD2)</f>
+        <v/>
+      </c>
+      <c r="AE2" t="str">
+        <f>IF(OR('Private Interp'!AE2="",'Public Interp'!AE2=""),"",'Private Interp'!AE2+'Public Interp'!AE2)</f>
+        <v/>
+      </c>
+      <c r="AF2" t="str">
+        <f>IF(OR('Private Interp'!AF2="",'Public Interp'!AF2=""),"",'Private Interp'!AF2+'Public Interp'!AF2)</f>
+        <v/>
+      </c>
+      <c r="AG2" t="str">
+        <f>IF(OR('Private Interp'!AG2="",'Public Interp'!AG2=""),"",'Private Interp'!AG2+'Public Interp'!AG2)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <f t="shared" ref="A4:A9" si="0">A3+1</f>
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>2005</v>
+      </c>
+      <c r="B7">
+        <f>IF(OR('Private Interp'!B7="",'Public Interp'!B7=""),"",'Private Interp'!B7+'Public Interp'!B7)</f>
+        <v>2.4670000000000001</v>
+      </c>
+      <c r="C7" t="str">
+        <f>IF(OR('Private Interp'!C7="",'Public Interp'!C7=""),"",'Private Interp'!C7+'Public Interp'!C7)</f>
+        <v/>
+      </c>
+      <c r="D7" t="str">
+        <f>IF(OR('Private Interp'!D7="",'Public Interp'!D7=""),"",'Private Interp'!D7+'Public Interp'!D7)</f>
+        <v/>
+      </c>
+      <c r="E7" t="str">
+        <f>IF(OR('Private Interp'!E7="",'Public Interp'!E7=""),"",'Private Interp'!E7+'Public Interp'!E7)</f>
+        <v/>
+      </c>
+      <c r="F7" t="str">
+        <f>IF(OR('Private Interp'!F7="",'Public Interp'!F7=""),"",'Private Interp'!F7+'Public Interp'!F7)</f>
+        <v/>
+      </c>
+      <c r="G7" t="str">
+        <f>IF(OR('Private Interp'!G7="",'Public Interp'!G7=""),"",'Private Interp'!G7+'Public Interp'!G7)</f>
+        <v/>
+      </c>
+      <c r="H7" t="str">
+        <f>IF(OR('Private Interp'!H7="",'Public Interp'!H7=""),"",'Private Interp'!H7+'Public Interp'!H7)</f>
+        <v/>
+      </c>
+      <c r="I7" t="str">
+        <f>IF(OR('Private Interp'!I7="",'Public Interp'!I7=""),"",'Private Interp'!I7+'Public Interp'!I7)</f>
+        <v/>
+      </c>
+      <c r="J7" t="str">
+        <f>IF(OR('Private Interp'!J7="",'Public Interp'!J7=""),"",'Private Interp'!J7+'Public Interp'!J7)</f>
+        <v/>
+      </c>
+      <c r="K7" t="str">
+        <f>IF(OR('Private Interp'!K7="",'Public Interp'!K7=""),"",'Private Interp'!K7+'Public Interp'!K7)</f>
+        <v/>
+      </c>
+      <c r="L7" t="str">
+        <f>IF(OR('Private Interp'!L7="",'Public Interp'!L7=""),"",'Private Interp'!L7+'Public Interp'!L7)</f>
+        <v/>
+      </c>
+      <c r="M7" t="str">
+        <f>IF(OR('Private Interp'!M7="",'Public Interp'!M7=""),"",'Private Interp'!M7+'Public Interp'!M7)</f>
+        <v/>
+      </c>
+      <c r="N7" t="str">
+        <f>IF(OR('Private Interp'!N7="",'Public Interp'!N7=""),"",'Private Interp'!N7+'Public Interp'!N7)</f>
+        <v/>
+      </c>
+      <c r="O7" t="str">
+        <f>IF(OR('Private Interp'!O7="",'Public Interp'!O7=""),"",'Private Interp'!O7+'Public Interp'!O7)</f>
+        <v/>
+      </c>
+      <c r="P7" t="str">
+        <f>IF(OR('Private Interp'!P7="",'Public Interp'!P7=""),"",'Private Interp'!P7+'Public Interp'!P7)</f>
+        <v/>
+      </c>
+      <c r="Q7" t="str">
+        <f>IF(OR('Private Interp'!Q7="",'Public Interp'!Q7=""),"",'Private Interp'!Q7+'Public Interp'!Q7)</f>
+        <v/>
+      </c>
+      <c r="R7" t="str">
+        <f>IF(OR('Private Interp'!R7="",'Public Interp'!R7=""),"",'Private Interp'!R7+'Public Interp'!R7)</f>
+        <v/>
+      </c>
+      <c r="S7" t="str">
+        <f>IF(OR('Private Interp'!S7="",'Public Interp'!S7=""),"",'Private Interp'!S7+'Public Interp'!S7)</f>
+        <v/>
+      </c>
+      <c r="T7" t="str">
+        <f>IF(OR('Private Interp'!T7="",'Public Interp'!T7=""),"",'Private Interp'!T7+'Public Interp'!T7)</f>
+        <v/>
+      </c>
+      <c r="U7" t="str">
+        <f>IF(OR('Private Interp'!U7="",'Public Interp'!U7=""),"",'Private Interp'!U7+'Public Interp'!U7)</f>
+        <v/>
+      </c>
+      <c r="V7" t="str">
+        <f>IF(OR('Private Interp'!V7="",'Public Interp'!V7=""),"",'Private Interp'!V7+'Public Interp'!V7)</f>
+        <v/>
+      </c>
+      <c r="W7" t="str">
+        <f>IF(OR('Private Interp'!W7="",'Public Interp'!W7=""),"",'Private Interp'!W7+'Public Interp'!W7)</f>
+        <v/>
+      </c>
+      <c r="X7" t="str">
+        <f>IF(OR('Private Interp'!X7="",'Public Interp'!X7=""),"",'Private Interp'!X7+'Public Interp'!X7)</f>
+        <v/>
+      </c>
+      <c r="Y7" t="str">
+        <f>IF(OR('Private Interp'!Y7="",'Public Interp'!Y7=""),"",'Private Interp'!Y7+'Public Interp'!Y7)</f>
+        <v/>
+      </c>
+      <c r="Z7" t="str">
+        <f>IF(OR('Private Interp'!Z7="",'Public Interp'!Z7=""),"",'Private Interp'!Z7+'Public Interp'!Z7)</f>
+        <v/>
+      </c>
+      <c r="AA7" t="str">
+        <f>IF(OR('Private Interp'!AA7="",'Public Interp'!AA7=""),"",'Private Interp'!AA7+'Public Interp'!AA7)</f>
+        <v/>
+      </c>
+      <c r="AB7" t="str">
+        <f>IF(OR('Private Interp'!AB7="",'Public Interp'!AB7=""),"",'Private Interp'!AB7+'Public Interp'!AB7)</f>
+        <v/>
+      </c>
+      <c r="AC7" t="str">
+        <f>IF(OR('Private Interp'!AC7="",'Public Interp'!AC7=""),"",'Private Interp'!AC7+'Public Interp'!AC7)</f>
+        <v/>
+      </c>
+      <c r="AD7" t="str">
+        <f>IF(OR('Private Interp'!AD7="",'Public Interp'!AD7=""),"",'Private Interp'!AD7+'Public Interp'!AD7)</f>
+        <v/>
+      </c>
+      <c r="AE7" t="str">
+        <f>IF(OR('Private Interp'!AE7="",'Public Interp'!AE7=""),"",'Private Interp'!AE7+'Public Interp'!AE7)</f>
+        <v/>
+      </c>
+      <c r="AF7" t="str">
+        <f>IF(OR('Private Interp'!AF7="",'Public Interp'!AF7=""),"",'Private Interp'!AF7+'Public Interp'!AF7)</f>
+        <v/>
+      </c>
+      <c r="AG7" t="str">
+        <f>IF(OR('Private Interp'!AG7="",'Public Interp'!AG7=""),"",'Private Interp'!AG7+'Public Interp'!AG7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>2008</v>
+      </c>
+      <c r="B10">
+        <f>IF(OR('Private Interp'!B10="",'Public Interp'!B10=""),"",'Private Interp'!B10+'Public Interp'!B10)</f>
+        <v>2.4239999999999999</v>
+      </c>
+      <c r="C10" t="str">
+        <f>IF(OR('Private Interp'!C10="",'Public Interp'!C10=""),"",'Private Interp'!C10+'Public Interp'!C10)</f>
+        <v/>
+      </c>
+      <c r="D10" t="str">
+        <f>IF(OR('Private Interp'!D10="",'Public Interp'!D10=""),"",'Private Interp'!D10+'Public Interp'!D10)</f>
+        <v/>
+      </c>
+      <c r="E10" t="str">
+        <f>IF(OR('Private Interp'!E10="",'Public Interp'!E10=""),"",'Private Interp'!E10+'Public Interp'!E10)</f>
+        <v/>
+      </c>
+      <c r="F10" t="str">
+        <f>IF(OR('Private Interp'!F10="",'Public Interp'!F10=""),"",'Private Interp'!F10+'Public Interp'!F10)</f>
+        <v/>
+      </c>
+      <c r="G10" t="str">
+        <f>IF(OR('Private Interp'!G10="",'Public Interp'!G10=""),"",'Private Interp'!G10+'Public Interp'!G10)</f>
+        <v/>
+      </c>
+      <c r="H10" t="str">
+        <f>IF(OR('Private Interp'!H10="",'Public Interp'!H10=""),"",'Private Interp'!H10+'Public Interp'!H10)</f>
+        <v/>
+      </c>
+      <c r="I10" t="str">
+        <f>IF(OR('Private Interp'!I10="",'Public Interp'!I10=""),"",'Private Interp'!I10+'Public Interp'!I10)</f>
+        <v/>
+      </c>
+      <c r="J10" t="str">
+        <f>IF(OR('Private Interp'!J10="",'Public Interp'!J10=""),"",'Private Interp'!J10+'Public Interp'!J10)</f>
+        <v/>
+      </c>
+      <c r="K10" t="str">
+        <f>IF(OR('Private Interp'!K10="",'Public Interp'!K10=""),"",'Private Interp'!K10+'Public Interp'!K10)</f>
+        <v/>
+      </c>
+      <c r="L10" t="str">
+        <f>IF(OR('Private Interp'!L10="",'Public Interp'!L10=""),"",'Private Interp'!L10+'Public Interp'!L10)</f>
+        <v/>
+      </c>
+      <c r="M10" t="str">
+        <f>IF(OR('Private Interp'!M10="",'Public Interp'!M10=""),"",'Private Interp'!M10+'Public Interp'!M10)</f>
+        <v/>
+      </c>
+      <c r="N10" t="str">
+        <f>IF(OR('Private Interp'!N10="",'Public Interp'!N10=""),"",'Private Interp'!N10+'Public Interp'!N10)</f>
+        <v/>
+      </c>
+      <c r="O10" t="str">
+        <f>IF(OR('Private Interp'!O10="",'Public Interp'!O10=""),"",'Private Interp'!O10+'Public Interp'!O10)</f>
+        <v/>
+      </c>
+      <c r="P10" t="str">
+        <f>IF(OR('Private Interp'!P10="",'Public Interp'!P10=""),"",'Private Interp'!P10+'Public Interp'!P10)</f>
+        <v/>
+      </c>
+      <c r="Q10" t="str">
+        <f>IF(OR('Private Interp'!Q10="",'Public Interp'!Q10=""),"",'Private Interp'!Q10+'Public Interp'!Q10)</f>
+        <v/>
+      </c>
+      <c r="R10" t="str">
+        <f>IF(OR('Private Interp'!R10="",'Public Interp'!R10=""),"",'Private Interp'!R10+'Public Interp'!R10)</f>
+        <v/>
+      </c>
+      <c r="S10" t="str">
+        <f>IF(OR('Private Interp'!S10="",'Public Interp'!S10=""),"",'Private Interp'!S10+'Public Interp'!S10)</f>
+        <v/>
+      </c>
+      <c r="T10" t="str">
+        <f>IF(OR('Private Interp'!T10="",'Public Interp'!T10=""),"",'Private Interp'!T10+'Public Interp'!T10)</f>
+        <v/>
+      </c>
+      <c r="U10" t="str">
+        <f>IF(OR('Private Interp'!U10="",'Public Interp'!U10=""),"",'Private Interp'!U10+'Public Interp'!U10)</f>
+        <v/>
+      </c>
+      <c r="V10" t="str">
+        <f>IF(OR('Private Interp'!V10="",'Public Interp'!V10=""),"",'Private Interp'!V10+'Public Interp'!V10)</f>
+        <v/>
+      </c>
+      <c r="W10" t="str">
+        <f>IF(OR('Private Interp'!W10="",'Public Interp'!W10=""),"",'Private Interp'!W10+'Public Interp'!W10)</f>
+        <v/>
+      </c>
+      <c r="X10" t="str">
+        <f>IF(OR('Private Interp'!X10="",'Public Interp'!X10=""),"",'Private Interp'!X10+'Public Interp'!X10)</f>
+        <v/>
+      </c>
+      <c r="Y10" t="str">
+        <f>IF(OR('Private Interp'!Y10="",'Public Interp'!Y10=""),"",'Private Interp'!Y10+'Public Interp'!Y10)</f>
+        <v/>
+      </c>
+      <c r="Z10" t="str">
+        <f>IF(OR('Private Interp'!Z10="",'Public Interp'!Z10=""),"",'Private Interp'!Z10+'Public Interp'!Z10)</f>
+        <v/>
+      </c>
+      <c r="AA10" t="str">
+        <f>IF(OR('Private Interp'!AA10="",'Public Interp'!AA10=""),"",'Private Interp'!AA10+'Public Interp'!AA10)</f>
+        <v/>
+      </c>
+      <c r="AB10" t="str">
+        <f>IF(OR('Private Interp'!AB10="",'Public Interp'!AB10=""),"",'Private Interp'!AB10+'Public Interp'!AB10)</f>
+        <v/>
+      </c>
+      <c r="AC10" t="str">
+        <f>IF(OR('Private Interp'!AC10="",'Public Interp'!AC10=""),"",'Private Interp'!AC10+'Public Interp'!AC10)</f>
+        <v/>
+      </c>
+      <c r="AD10" t="str">
+        <f>IF(OR('Private Interp'!AD10="",'Public Interp'!AD10=""),"",'Private Interp'!AD10+'Public Interp'!AD10)</f>
+        <v/>
+      </c>
+      <c r="AE10" t="str">
+        <f>IF(OR('Private Interp'!AE10="",'Public Interp'!AE10=""),"",'Private Interp'!AE10+'Public Interp'!AE10)</f>
+        <v/>
+      </c>
+      <c r="AF10" t="str">
+        <f>IF(OR('Private Interp'!AF10="",'Public Interp'!AF10=""),"",'Private Interp'!AF10+'Public Interp'!AF10)</f>
+        <v/>
+      </c>
+      <c r="AG10" t="str">
+        <f>IF(OR('Private Interp'!AG10="",'Public Interp'!AG10=""),"",'Private Interp'!AG10+'Public Interp'!AG10)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>2009</v>
+      </c>
+      <c r="B11">
+        <f>IF(OR('Private Interp'!B11="",'Public Interp'!B11=""),"",'Private Interp'!B11+'Public Interp'!B11)</f>
+        <v>2.5640000000000001</v>
+      </c>
+      <c r="C11" t="str">
+        <f>IF(OR('Private Interp'!C11="",'Public Interp'!C11=""),"",'Private Interp'!C11+'Public Interp'!C11)</f>
+        <v/>
+      </c>
+      <c r="D11" t="str">
+        <f>IF(OR('Private Interp'!D11="",'Public Interp'!D11=""),"",'Private Interp'!D11+'Public Interp'!D11)</f>
+        <v/>
+      </c>
+      <c r="E11" t="str">
+        <f>IF(OR('Private Interp'!E11="",'Public Interp'!E11=""),"",'Private Interp'!E11+'Public Interp'!E11)</f>
+        <v/>
+      </c>
+      <c r="F11" t="str">
+        <f>IF(OR('Private Interp'!F11="",'Public Interp'!F11=""),"",'Private Interp'!F11+'Public Interp'!F11)</f>
+        <v/>
+      </c>
+      <c r="G11" t="str">
+        <f>IF(OR('Private Interp'!G11="",'Public Interp'!G11=""),"",'Private Interp'!G11+'Public Interp'!G11)</f>
+        <v/>
+      </c>
+      <c r="H11" t="str">
+        <f>IF(OR('Private Interp'!H11="",'Public Interp'!H11=""),"",'Private Interp'!H11+'Public Interp'!H11)</f>
+        <v/>
+      </c>
+      <c r="I11" t="str">
+        <f>IF(OR('Private Interp'!I11="",'Public Interp'!I11=""),"",'Private Interp'!I11+'Public Interp'!I11)</f>
+        <v/>
+      </c>
+      <c r="J11" t="str">
+        <f>IF(OR('Private Interp'!J11="",'Public Interp'!J11=""),"",'Private Interp'!J11+'Public Interp'!J11)</f>
+        <v/>
+      </c>
+      <c r="K11" t="str">
+        <f>IF(OR('Private Interp'!K11="",'Public Interp'!K11=""),"",'Private Interp'!K11+'Public Interp'!K11)</f>
+        <v/>
+      </c>
+      <c r="L11" t="str">
+        <f>IF(OR('Private Interp'!L11="",'Public Interp'!L11=""),"",'Private Interp'!L11+'Public Interp'!L11)</f>
+        <v/>
+      </c>
+      <c r="M11" t="str">
+        <f>IF(OR('Private Interp'!M11="",'Public Interp'!M11=""),"",'Private Interp'!M11+'Public Interp'!M11)</f>
+        <v/>
+      </c>
+      <c r="N11" t="str">
+        <f>IF(OR('Private Interp'!N11="",'Public Interp'!N11=""),"",'Private Interp'!N11+'Public Interp'!N11)</f>
+        <v/>
+      </c>
+      <c r="O11" t="str">
+        <f>IF(OR('Private Interp'!O11="",'Public Interp'!O11=""),"",'Private Interp'!O11+'Public Interp'!O11)</f>
+        <v/>
+      </c>
+      <c r="P11" t="str">
+        <f>IF(OR('Private Interp'!P11="",'Public Interp'!P11=""),"",'Private Interp'!P11+'Public Interp'!P11)</f>
+        <v/>
+      </c>
+      <c r="Q11" t="str">
+        <f>IF(OR('Private Interp'!Q11="",'Public Interp'!Q11=""),"",'Private Interp'!Q11+'Public Interp'!Q11)</f>
+        <v/>
+      </c>
+      <c r="R11" t="str">
+        <f>IF(OR('Private Interp'!R11="",'Public Interp'!R11=""),"",'Private Interp'!R11+'Public Interp'!R11)</f>
+        <v/>
+      </c>
+      <c r="S11" t="str">
+        <f>IF(OR('Private Interp'!S11="",'Public Interp'!S11=""),"",'Private Interp'!S11+'Public Interp'!S11)</f>
+        <v/>
+      </c>
+      <c r="T11" t="str">
+        <f>IF(OR('Private Interp'!T11="",'Public Interp'!T11=""),"",'Private Interp'!T11+'Public Interp'!T11)</f>
+        <v/>
+      </c>
+      <c r="U11" t="str">
+        <f>IF(OR('Private Interp'!U11="",'Public Interp'!U11=""),"",'Private Interp'!U11+'Public Interp'!U11)</f>
+        <v/>
+      </c>
+      <c r="V11" t="str">
+        <f>IF(OR('Private Interp'!V11="",'Public Interp'!V11=""),"",'Private Interp'!V11+'Public Interp'!V11)</f>
+        <v/>
+      </c>
+      <c r="W11" t="str">
+        <f>IF(OR('Private Interp'!W11="",'Public Interp'!W11=""),"",'Private Interp'!W11+'Public Interp'!W11)</f>
+        <v/>
+      </c>
+      <c r="X11" t="str">
+        <f>IF(OR('Private Interp'!X11="",'Public Interp'!X11=""),"",'Private Interp'!X11+'Public Interp'!X11)</f>
+        <v/>
+      </c>
+      <c r="Y11" t="str">
+        <f>IF(OR('Private Interp'!Y11="",'Public Interp'!Y11=""),"",'Private Interp'!Y11+'Public Interp'!Y11)</f>
+        <v/>
+      </c>
+      <c r="Z11" t="str">
+        <f>IF(OR('Private Interp'!Z11="",'Public Interp'!Z11=""),"",'Private Interp'!Z11+'Public Interp'!Z11)</f>
+        <v/>
+      </c>
+      <c r="AA11" t="str">
+        <f>IF(OR('Private Interp'!AA11="",'Public Interp'!AA11=""),"",'Private Interp'!AA11+'Public Interp'!AA11)</f>
+        <v/>
+      </c>
+      <c r="AB11" t="str">
+        <f>IF(OR('Private Interp'!AB11="",'Public Interp'!AB11=""),"",'Private Interp'!AB11+'Public Interp'!AB11)</f>
+        <v/>
+      </c>
+      <c r="AC11" t="str">
+        <f>IF(OR('Private Interp'!AC11="",'Public Interp'!AC11=""),"",'Private Interp'!AC11+'Public Interp'!AC11)</f>
+        <v/>
+      </c>
+      <c r="AD11" t="str">
+        <f>IF(OR('Private Interp'!AD11="",'Public Interp'!AD11=""),"",'Private Interp'!AD11+'Public Interp'!AD11)</f>
+        <v/>
+      </c>
+      <c r="AE11" t="str">
+        <f>IF(OR('Private Interp'!AE11="",'Public Interp'!AE11=""),"",'Private Interp'!AE11+'Public Interp'!AE11)</f>
+        <v/>
+      </c>
+      <c r="AF11" t="str">
+        <f>IF(OR('Private Interp'!AF11="",'Public Interp'!AF11=""),"",'Private Interp'!AF11+'Public Interp'!AF11)</f>
+        <v/>
+      </c>
+      <c r="AG11" t="str">
+        <f>IF(OR('Private Interp'!AG11="",'Public Interp'!AG11=""),"",'Private Interp'!AG11+'Public Interp'!AG11)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>2010</v>
+      </c>
+      <c r="B12">
+        <f>IF(OR('Private Interp'!B12="",'Public Interp'!B12=""),"",'Private Interp'!B12+'Public Interp'!B12)</f>
+        <v>2.665</v>
+      </c>
+      <c r="C12" t="str">
+        <f>IF(OR('Private Interp'!C12="",'Public Interp'!C12=""),"",'Private Interp'!C12+'Public Interp'!C12)</f>
+        <v/>
+      </c>
+      <c r="D12" t="str">
+        <f>IF(OR('Private Interp'!D12="",'Public Interp'!D12=""),"",'Private Interp'!D12+'Public Interp'!D12)</f>
+        <v/>
+      </c>
+      <c r="E12" t="str">
+        <f>IF(OR('Private Interp'!E12="",'Public Interp'!E12=""),"",'Private Interp'!E12+'Public Interp'!E12)</f>
+        <v/>
+      </c>
+      <c r="F12" t="str">
+        <f>IF(OR('Private Interp'!F12="",'Public Interp'!F12=""),"",'Private Interp'!F12+'Public Interp'!F12)</f>
+        <v/>
+      </c>
+      <c r="G12" t="str">
+        <f>IF(OR('Private Interp'!G12="",'Public Interp'!G12=""),"",'Private Interp'!G12+'Public Interp'!G12)</f>
+        <v/>
+      </c>
+      <c r="H12" t="str">
+        <f>IF(OR('Private Interp'!H12="",'Public Interp'!H12=""),"",'Private Interp'!H12+'Public Interp'!H12)</f>
+        <v/>
+      </c>
+      <c r="I12" t="str">
+        <f>IF(OR('Private Interp'!I12="",'Public Interp'!I12=""),"",'Private Interp'!I12+'Public Interp'!I12)</f>
+        <v/>
+      </c>
+      <c r="J12" t="str">
+        <f>IF(OR('Private Interp'!J12="",'Public Interp'!J12=""),"",'Private Interp'!J12+'Public Interp'!J12)</f>
+        <v/>
+      </c>
+      <c r="K12" t="str">
+        <f>IF(OR('Private Interp'!K12="",'Public Interp'!K12=""),"",'Private Interp'!K12+'Public Interp'!K12)</f>
+        <v/>
+      </c>
+      <c r="L12" t="str">
+        <f>IF(OR('Private Interp'!L12="",'Public Interp'!L12=""),"",'Private Interp'!L12+'Public Interp'!L12)</f>
+        <v/>
+      </c>
+      <c r="M12" t="str">
+        <f>IF(OR('Private Interp'!M12="",'Public Interp'!M12=""),"",'Private Interp'!M12+'Public Interp'!M12)</f>
+        <v/>
+      </c>
+      <c r="N12" t="str">
+        <f>IF(OR('Private Interp'!N12="",'Public Interp'!N12=""),"",'Private Interp'!N12+'Public Interp'!N12)</f>
+        <v/>
+      </c>
+      <c r="O12" t="str">
+        <f>IF(OR('Private Interp'!O12="",'Public Interp'!O12=""),"",'Private Interp'!O12+'Public Interp'!O12)</f>
+        <v/>
+      </c>
+      <c r="P12" t="str">
+        <f>IF(OR('Private Interp'!P12="",'Public Interp'!P12=""),"",'Private Interp'!P12+'Public Interp'!P12)</f>
+        <v/>
+      </c>
+      <c r="Q12" t="str">
+        <f>IF(OR('Private Interp'!Q12="",'Public Interp'!Q12=""),"",'Private Interp'!Q12+'Public Interp'!Q12)</f>
+        <v/>
+      </c>
+      <c r="R12" t="str">
+        <f>IF(OR('Private Interp'!R12="",'Public Interp'!R12=""),"",'Private Interp'!R12+'Public Interp'!R12)</f>
+        <v/>
+      </c>
+      <c r="S12" t="str">
+        <f>IF(OR('Private Interp'!S12="",'Public Interp'!S12=""),"",'Private Interp'!S12+'Public Interp'!S12)</f>
+        <v/>
+      </c>
+      <c r="T12" t="str">
+        <f>IF(OR('Private Interp'!T12="",'Public Interp'!T12=""),"",'Private Interp'!T12+'Public Interp'!T12)</f>
+        <v/>
+      </c>
+      <c r="U12" t="str">
+        <f>IF(OR('Private Interp'!U12="",'Public Interp'!U12=""),"",'Private Interp'!U12+'Public Interp'!U12)</f>
+        <v/>
+      </c>
+      <c r="V12" t="str">
+        <f>IF(OR('Private Interp'!V12="",'Public Interp'!V12=""),"",'Private Interp'!V12+'Public Interp'!V12)</f>
+        <v/>
+      </c>
+      <c r="W12" t="str">
+        <f>IF(OR('Private Interp'!W12="",'Public Interp'!W12=""),"",'Private Interp'!W12+'Public Interp'!W12)</f>
+        <v/>
+      </c>
+      <c r="X12" t="str">
+        <f>IF(OR('Private Interp'!X12="",'Public Interp'!X12=""),"",'Private Interp'!X12+'Public Interp'!X12)</f>
+        <v/>
+      </c>
+      <c r="Y12" t="str">
+        <f>IF(OR('Private Interp'!Y12="",'Public Interp'!Y12=""),"",'Private Interp'!Y12+'Public Interp'!Y12)</f>
+        <v/>
+      </c>
+      <c r="Z12" t="str">
+        <f>IF(OR('Private Interp'!Z12="",'Public Interp'!Z12=""),"",'Private Interp'!Z12+'Public Interp'!Z12)</f>
+        <v/>
+      </c>
+      <c r="AA12" t="str">
+        <f>IF(OR('Private Interp'!AA12="",'Public Interp'!AA12=""),"",'Private Interp'!AA12+'Public Interp'!AA12)</f>
+        <v/>
+      </c>
+      <c r="AB12" t="str">
+        <f>IF(OR('Private Interp'!AB12="",'Public Interp'!AB12=""),"",'Private Interp'!AB12+'Public Interp'!AB12)</f>
+        <v/>
+      </c>
+      <c r="AC12" t="str">
+        <f>IF(OR('Private Interp'!AC12="",'Public Interp'!AC12=""),"",'Private Interp'!AC12+'Public Interp'!AC12)</f>
+        <v/>
+      </c>
+      <c r="AD12" t="str">
+        <f>IF(OR('Private Interp'!AD12="",'Public Interp'!AD12=""),"",'Private Interp'!AD12+'Public Interp'!AD12)</f>
+        <v/>
+      </c>
+      <c r="AE12" t="str">
+        <f>IF(OR('Private Interp'!AE12="",'Public Interp'!AE12=""),"",'Private Interp'!AE12+'Public Interp'!AE12)</f>
+        <v/>
+      </c>
+      <c r="AF12" t="str">
+        <f>IF(OR('Private Interp'!AF12="",'Public Interp'!AF12=""),"",'Private Interp'!AF12+'Public Interp'!AF12)</f>
+        <v/>
+      </c>
+      <c r="AG12" t="str">
+        <f>IF(OR('Private Interp'!AG12="",'Public Interp'!AG12=""),"",'Private Interp'!AG12+'Public Interp'!AG12)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>2011</v>
+      </c>
+      <c r="B13">
+        <f>IF(OR('Private Interp'!B13="",'Public Interp'!B13=""),"",'Private Interp'!B13+'Public Interp'!B13)</f>
+        <v>2.5840000000000001</v>
+      </c>
+      <c r="C13">
+        <f>IF(OR('Private Interp'!C13="",'Public Interp'!C13=""),"",'Private Interp'!C13+'Public Interp'!C13)</f>
+        <v>3.9269999999999996</v>
+      </c>
+      <c r="D13">
+        <f>IF(OR('Private Interp'!D13="",'Public Interp'!D13=""),"",'Private Interp'!D13+'Public Interp'!D13)</f>
+        <v>2.3051040713961113</v>
+      </c>
+      <c r="E13">
+        <f>IF(OR('Private Interp'!E13="",'Public Interp'!E13=""),"",'Private Interp'!E13+'Public Interp'!E13)</f>
+        <v>3.1434192897479538</v>
+      </c>
+      <c r="F13">
+        <f>IF(OR('Private Interp'!F13="",'Public Interp'!F13=""),"",'Private Interp'!F13+'Public Interp'!F13)</f>
+        <v>2.5503240153640712</v>
+      </c>
+      <c r="G13" t="str">
+        <f>IF(OR('Private Interp'!G13="",'Public Interp'!G13=""),"",'Private Interp'!G13+'Public Interp'!G13)</f>
+        <v/>
+      </c>
+      <c r="H13" t="str">
+        <f>IF(OR('Private Interp'!H13="",'Public Interp'!H13=""),"",'Private Interp'!H13+'Public Interp'!H13)</f>
+        <v/>
+      </c>
+      <c r="I13" t="str">
+        <f>IF(OR('Private Interp'!I13="",'Public Interp'!I13=""),"",'Private Interp'!I13+'Public Interp'!I13)</f>
+        <v/>
+      </c>
+      <c r="J13" t="str">
+        <f>IF(OR('Private Interp'!J13="",'Public Interp'!J13=""),"",'Private Interp'!J13+'Public Interp'!J13)</f>
+        <v/>
+      </c>
+      <c r="K13" t="str">
+        <f>IF(OR('Private Interp'!K13="",'Public Interp'!K13=""),"",'Private Interp'!K13+'Public Interp'!K13)</f>
+        <v/>
+      </c>
+      <c r="L13" t="str">
+        <f>IF(OR('Private Interp'!L13="",'Public Interp'!L13=""),"",'Private Interp'!L13+'Public Interp'!L13)</f>
+        <v/>
+      </c>
+      <c r="M13" t="str">
+        <f>IF(OR('Private Interp'!M13="",'Public Interp'!M13=""),"",'Private Interp'!M13+'Public Interp'!M13)</f>
+        <v/>
+      </c>
+      <c r="N13" t="str">
+        <f>IF(OR('Private Interp'!N13="",'Public Interp'!N13=""),"",'Private Interp'!N13+'Public Interp'!N13)</f>
+        <v/>
+      </c>
+      <c r="O13" t="str">
+        <f>IF(OR('Private Interp'!O13="",'Public Interp'!O13=""),"",'Private Interp'!O13+'Public Interp'!O13)</f>
+        <v/>
+      </c>
+      <c r="P13" t="str">
+        <f>IF(OR('Private Interp'!P13="",'Public Interp'!P13=""),"",'Private Interp'!P13+'Public Interp'!P13)</f>
+        <v/>
+      </c>
+      <c r="Q13" t="str">
+        <f>IF(OR('Private Interp'!Q13="",'Public Interp'!Q13=""),"",'Private Interp'!Q13+'Public Interp'!Q13)</f>
+        <v/>
+      </c>
+      <c r="R13" t="str">
+        <f>IF(OR('Private Interp'!R13="",'Public Interp'!R13=""),"",'Private Interp'!R13+'Public Interp'!R13)</f>
+        <v/>
+      </c>
+      <c r="S13" t="str">
+        <f>IF(OR('Private Interp'!S13="",'Public Interp'!S13=""),"",'Private Interp'!S13+'Public Interp'!S13)</f>
+        <v/>
+      </c>
+      <c r="T13" t="str">
+        <f>IF(OR('Private Interp'!T13="",'Public Interp'!T13=""),"",'Private Interp'!T13+'Public Interp'!T13)</f>
+        <v/>
+      </c>
+      <c r="U13" t="str">
+        <f>IF(OR('Private Interp'!U13="",'Public Interp'!U13=""),"",'Private Interp'!U13+'Public Interp'!U13)</f>
+        <v/>
+      </c>
+      <c r="V13" t="str">
+        <f>IF(OR('Private Interp'!V13="",'Public Interp'!V13=""),"",'Private Interp'!V13+'Public Interp'!V13)</f>
+        <v/>
+      </c>
+      <c r="W13" t="str">
+        <f>IF(OR('Private Interp'!W13="",'Public Interp'!W13=""),"",'Private Interp'!W13+'Public Interp'!W13)</f>
+        <v/>
+      </c>
+      <c r="X13" t="str">
+        <f>IF(OR('Private Interp'!X13="",'Public Interp'!X13=""),"",'Private Interp'!X13+'Public Interp'!X13)</f>
+        <v/>
+      </c>
+      <c r="Y13" t="str">
+        <f>IF(OR('Private Interp'!Y13="",'Public Interp'!Y13=""),"",'Private Interp'!Y13+'Public Interp'!Y13)</f>
+        <v/>
+      </c>
+      <c r="Z13" t="str">
+        <f>IF(OR('Private Interp'!Z13="",'Public Interp'!Z13=""),"",'Private Interp'!Z13+'Public Interp'!Z13)</f>
+        <v/>
+      </c>
+      <c r="AA13" t="str">
+        <f>IF(OR('Private Interp'!AA13="",'Public Interp'!AA13=""),"",'Private Interp'!AA13+'Public Interp'!AA13)</f>
+        <v/>
+      </c>
+      <c r="AB13" t="str">
+        <f>IF(OR('Private Interp'!AB13="",'Public Interp'!AB13=""),"",'Private Interp'!AB13+'Public Interp'!AB13)</f>
+        <v/>
+      </c>
+      <c r="AC13" t="str">
+        <f>IF(OR('Private Interp'!AC13="",'Public Interp'!AC13=""),"",'Private Interp'!AC13+'Public Interp'!AC13)</f>
+        <v/>
+      </c>
+      <c r="AD13" t="str">
+        <f>IF(OR('Private Interp'!AD13="",'Public Interp'!AD13=""),"",'Private Interp'!AD13+'Public Interp'!AD13)</f>
+        <v/>
+      </c>
+      <c r="AE13" t="str">
+        <f>IF(OR('Private Interp'!AE13="",'Public Interp'!AE13=""),"",'Private Interp'!AE13+'Public Interp'!AE13)</f>
+        <v/>
+      </c>
+      <c r="AF13" t="str">
+        <f>IF(OR('Private Interp'!AF13="",'Public Interp'!AF13=""),"",'Private Interp'!AF13+'Public Interp'!AF13)</f>
+        <v/>
+      </c>
+      <c r="AG13">
+        <f>IF(OR('Private Interp'!AG13="",'Public Interp'!AG13=""),"",'Private Interp'!AG13+'Public Interp'!AG13)</f>
+        <v>3.6909999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>2012</v>
+      </c>
+      <c r="B14">
+        <f>IF(OR('Private Interp'!B14="",'Public Interp'!B14=""),"",'Private Interp'!B14+'Public Interp'!B14)</f>
+        <v>2.5350000000000001</v>
+      </c>
+      <c r="C14">
+        <f>IF(OR('Private Interp'!C14="",'Public Interp'!C14=""),"",'Private Interp'!C14+'Public Interp'!C14)</f>
+        <v>3.9249999999999998</v>
+      </c>
+      <c r="D14">
+        <f>IF(OR('Private Interp'!D14="",'Public Interp'!D14=""),"",'Private Interp'!D14+'Public Interp'!D14)</f>
+        <v>2.3079999999999998</v>
+      </c>
+      <c r="E14">
+        <f>IF(OR('Private Interp'!E14="",'Public Interp'!E14=""),"",'Private Interp'!E14+'Public Interp'!E14)</f>
+        <v>3.0960000000000001</v>
+      </c>
+      <c r="F14">
+        <f>IF(OR('Private Interp'!F14="",'Public Interp'!F14=""),"",'Private Interp'!F14+'Public Interp'!F14)</f>
+        <v>2.569</v>
+      </c>
+      <c r="G14" t="str">
+        <f>IF(OR('Private Interp'!G14="",'Public Interp'!G14=""),"",'Private Interp'!G14+'Public Interp'!G14)</f>
+        <v/>
+      </c>
+      <c r="H14">
+        <f>IF(OR('Private Interp'!H14="",'Public Interp'!H14=""),"",'Private Interp'!H14+'Public Interp'!H14)</f>
+        <v>-3.4048629324889335E-2</v>
+      </c>
+      <c r="I14">
+        <f>IF(OR('Private Interp'!I14="",'Public Interp'!I14=""),"",'Private Interp'!I14+'Public Interp'!I14)</f>
+        <v>2.139956322482639E-2</v>
+      </c>
+      <c r="J14" t="str">
+        <f>IF(OR('Private Interp'!J14="",'Public Interp'!J14=""),"",'Private Interp'!J14+'Public Interp'!J14)</f>
+        <v/>
+      </c>
+      <c r="K14" t="str">
+        <f>IF(OR('Private Interp'!K14="",'Public Interp'!K14=""),"",'Private Interp'!K14+'Public Interp'!K14)</f>
+        <v/>
+      </c>
+      <c r="L14">
+        <f>IF(OR('Private Interp'!L14="",'Public Interp'!L14=""),"",'Private Interp'!L14+'Public Interp'!L14)</f>
+        <v>2.4579857074047279E-2</v>
+      </c>
+      <c r="M14">
+        <f>IF(OR('Private Interp'!M14="",'Public Interp'!M14=""),"",'Private Interp'!M14+'Public Interp'!M14)</f>
+        <v>0.19810739755079754</v>
+      </c>
+      <c r="N14">
+        <f>IF(OR('Private Interp'!N14="",'Public Interp'!N14=""),"",'Private Interp'!N14+'Public Interp'!N14)</f>
+        <v>3.0932824499456637</v>
+      </c>
+      <c r="O14">
+        <f>IF(OR('Private Interp'!O14="",'Public Interp'!O14=""),"",'Private Interp'!O14+'Public Interp'!O14)</f>
+        <v>2.7640000000000002</v>
+      </c>
+      <c r="P14">
+        <f>IF(OR('Private Interp'!P14="",'Public Interp'!P14=""),"",'Private Interp'!P14+'Public Interp'!P14)</f>
+        <v>3.653</v>
+      </c>
+      <c r="Q14">
+        <f>IF(OR('Private Interp'!Q14="",'Public Interp'!Q14=""),"",'Private Interp'!Q14+'Public Interp'!Q14)</f>
+        <v>2.617</v>
+      </c>
+      <c r="R14">
+        <f>IF(OR('Private Interp'!R14="",'Public Interp'!R14=""),"",'Private Interp'!R14+'Public Interp'!R14)</f>
+        <v>2.8149999999999999</v>
+      </c>
+      <c r="S14">
+        <f>IF(OR('Private Interp'!S14="",'Public Interp'!S14=""),"",'Private Interp'!S14+'Public Interp'!S14)</f>
+        <v>2.1110000000000002</v>
+      </c>
+      <c r="T14">
+        <f>IF(OR('Private Interp'!T14="",'Public Interp'!T14=""),"",'Private Interp'!T14+'Public Interp'!T14)</f>
+        <v>1.867</v>
+      </c>
+      <c r="U14" t="str">
+        <f>IF(OR('Private Interp'!U14="",'Public Interp'!U14=""),"",'Private Interp'!U14+'Public Interp'!U14)</f>
+        <v/>
+      </c>
+      <c r="V14" t="str">
+        <f>IF(OR('Private Interp'!V14="",'Public Interp'!V14=""),"",'Private Interp'!V14+'Public Interp'!V14)</f>
+        <v/>
+      </c>
+      <c r="W14" t="str">
+        <f>IF(OR('Private Interp'!W14="",'Public Interp'!W14=""),"",'Private Interp'!W14+'Public Interp'!W14)</f>
+        <v/>
+      </c>
+      <c r="X14" t="str">
+        <f>IF(OR('Private Interp'!X14="",'Public Interp'!X14=""),"",'Private Interp'!X14+'Public Interp'!X14)</f>
+        <v/>
+      </c>
+      <c r="Y14" t="str">
+        <f>IF(OR('Private Interp'!Y14="",'Public Interp'!Y14=""),"",'Private Interp'!Y14+'Public Interp'!Y14)</f>
+        <v/>
+      </c>
+      <c r="Z14" t="str">
+        <f>IF(OR('Private Interp'!Z14="",'Public Interp'!Z14=""),"",'Private Interp'!Z14+'Public Interp'!Z14)</f>
+        <v/>
+      </c>
+      <c r="AA14" t="str">
+        <f>IF(OR('Private Interp'!AA14="",'Public Interp'!AA14=""),"",'Private Interp'!AA14+'Public Interp'!AA14)</f>
+        <v/>
+      </c>
+      <c r="AB14" t="str">
+        <f>IF(OR('Private Interp'!AB14="",'Public Interp'!AB14=""),"",'Private Interp'!AB14+'Public Interp'!AB14)</f>
+        <v/>
+      </c>
+      <c r="AC14" t="str">
+        <f>IF(OR('Private Interp'!AC14="",'Public Interp'!AC14=""),"",'Private Interp'!AC14+'Public Interp'!AC14)</f>
+        <v/>
+      </c>
+      <c r="AD14" t="str">
+        <f>IF(OR('Private Interp'!AD14="",'Public Interp'!AD14=""),"",'Private Interp'!AD14+'Public Interp'!AD14)</f>
+        <v/>
+      </c>
+      <c r="AE14" t="str">
+        <f>IF(OR('Private Interp'!AE14="",'Public Interp'!AE14=""),"",'Private Interp'!AE14+'Public Interp'!AE14)</f>
+        <v/>
+      </c>
+      <c r="AF14">
+        <f>IF(OR('Private Interp'!AF14="",'Public Interp'!AF14=""),"",'Private Interp'!AF14+'Public Interp'!AF14)</f>
+        <v>3.3040000000000003</v>
+      </c>
+      <c r="AG14">
+        <f>IF(OR('Private Interp'!AG14="",'Public Interp'!AG14=""),"",'Private Interp'!AG14+'Public Interp'!AG14)</f>
+        <v>3.714</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>2013</v>
+      </c>
+      <c r="B15">
+        <f>IF(OR('Private Interp'!B15="",'Public Interp'!B15=""),"",'Private Interp'!B15+'Public Interp'!B15)</f>
+        <v>2.5960000000000001</v>
+      </c>
+      <c r="C15">
+        <f>IF(OR('Private Interp'!C15="",'Public Interp'!C15=""),"",'Private Interp'!C15+'Public Interp'!C15)</f>
+        <v>3.931</v>
+      </c>
+      <c r="D15">
+        <f>IF(OR('Private Interp'!D15="",'Public Interp'!D15=""),"",'Private Interp'!D15+'Public Interp'!D15)</f>
+        <v>2.2789999999999999</v>
+      </c>
+      <c r="E15">
+        <f>IF(OR('Private Interp'!E15="",'Public Interp'!E15=""),"",'Private Interp'!E15+'Public Interp'!E15)</f>
+        <v>3.1720000000000002</v>
+      </c>
+      <c r="F15">
+        <f>IF(OR('Private Interp'!F15="",'Public Interp'!F15=""),"",'Private Interp'!F15+'Public Interp'!F15)</f>
+        <v>2.585561692425451</v>
+      </c>
+      <c r="G15" t="str">
+        <f>IF(OR('Private Interp'!G15="",'Public Interp'!G15=""),"",'Private Interp'!G15+'Public Interp'!G15)</f>
+        <v/>
+      </c>
+      <c r="H15">
+        <f>IF(OR('Private Interp'!H15="",'Public Interp'!H15=""),"",'Private Interp'!H15+'Public Interp'!H15)</f>
+        <v>5.9516837666003491E-2</v>
+      </c>
+      <c r="I15">
+        <f>IF(OR('Private Interp'!I15="",'Public Interp'!I15=""),"",'Private Interp'!I15+'Public Interp'!I15)</f>
+        <v>3.7137512398026096E-2</v>
+      </c>
+      <c r="J15">
+        <f>IF(OR('Private Interp'!J15="",'Public Interp'!J15=""),"",'Private Interp'!J15+'Public Interp'!J15)</f>
+        <v>-2.5287220712426228E-2</v>
+      </c>
+      <c r="K15">
+        <f>IF(OR('Private Interp'!K15="",'Public Interp'!K15=""),"",'Private Interp'!K15+'Public Interp'!K15)</f>
+        <v>5.6350568783376742E-2</v>
+      </c>
+      <c r="L15">
+        <f>IF(OR('Private Interp'!L15="",'Public Interp'!L15=""),"",'Private Interp'!L15+'Public Interp'!L15)</f>
+        <v>4.1991170523139186E-2</v>
+      </c>
+      <c r="M15">
+        <f>IF(OR('Private Interp'!M15="",'Public Interp'!M15=""),"",'Private Interp'!M15+'Public Interp'!M15)</f>
+        <v>0.21253983410546681</v>
+      </c>
+      <c r="N15">
+        <f>IF(OR('Private Interp'!N15="",'Public Interp'!N15=""),"",'Private Interp'!N15+'Public Interp'!N15)</f>
+        <v>3.1669999999999998</v>
+      </c>
+      <c r="O15">
+        <f>IF(OR('Private Interp'!O15="",'Public Interp'!O15=""),"",'Private Interp'!O15+'Public Interp'!O15)</f>
+        <v>2.8260000000000001</v>
+      </c>
+      <c r="P15">
+        <f>IF(OR('Private Interp'!P15="",'Public Interp'!P15=""),"",'Private Interp'!P15+'Public Interp'!P15)</f>
+        <v>3.5890000000000004</v>
+      </c>
+      <c r="Q15">
+        <f>IF(OR('Private Interp'!Q15="",'Public Interp'!Q15=""),"",'Private Interp'!Q15+'Public Interp'!Q15)</f>
+        <v>2.661</v>
+      </c>
+      <c r="R15">
+        <f>IF(OR('Private Interp'!R15="",'Public Interp'!R15=""),"",'Private Interp'!R15+'Public Interp'!R15)</f>
+        <v>2.698</v>
+      </c>
+      <c r="S15">
+        <f>IF(OR('Private Interp'!S15="",'Public Interp'!S15=""),"",'Private Interp'!S15+'Public Interp'!S15)</f>
+        <v>2.266</v>
+      </c>
+      <c r="T15">
+        <f>IF(OR('Private Interp'!T15="",'Public Interp'!T15=""),"",'Private Interp'!T15+'Public Interp'!T15)</f>
+        <v>1.857900440847388</v>
+      </c>
+      <c r="U15" t="str">
+        <f>IF(OR('Private Interp'!U15="",'Public Interp'!U15=""),"",'Private Interp'!U15+'Public Interp'!U15)</f>
+        <v/>
+      </c>
+      <c r="V15" t="str">
+        <f>IF(OR('Private Interp'!V15="",'Public Interp'!V15=""),"",'Private Interp'!V15+'Public Interp'!V15)</f>
+        <v/>
+      </c>
+      <c r="W15" t="str">
+        <f>IF(OR('Private Interp'!W15="",'Public Interp'!W15=""),"",'Private Interp'!W15+'Public Interp'!W15)</f>
+        <v/>
+      </c>
+      <c r="X15">
+        <f>IF(OR('Private Interp'!X15="",'Public Interp'!X15=""),"",'Private Interp'!X15+'Public Interp'!X15)</f>
+        <v>1.4378561170499404E-3</v>
+      </c>
+      <c r="Y15">
+        <f>IF(OR('Private Interp'!Y15="",'Public Interp'!Y15=""),"",'Private Interp'!Y15+'Public Interp'!Y15)</f>
+        <v>-4.1519935417142384E-2</v>
+      </c>
+      <c r="Z15">
+        <f>IF(OR('Private Interp'!Z15="",'Public Interp'!Z15=""),"",'Private Interp'!Z15+'Public Interp'!Z15)</f>
+        <v>1.5633808235725605E-2</v>
+      </c>
+      <c r="AA15">
+        <f>IF(OR('Private Interp'!AA15="",'Public Interp'!AA15=""),"",'Private Interp'!AA15+'Public Interp'!AA15)</f>
+        <v>-0.16050422716142151</v>
+      </c>
+      <c r="AB15">
+        <f>IF(OR('Private Interp'!AB15="",'Public Interp'!AB15=""),"",'Private Interp'!AB15+'Public Interp'!AB15)</f>
+        <v>0.18156645738110355</v>
+      </c>
+      <c r="AC15">
+        <f>IF(OR('Private Interp'!AC15="",'Public Interp'!AC15=""),"",'Private Interp'!AC15+'Public Interp'!AC15)</f>
+        <v>-1.6283065843117277E-2</v>
+      </c>
+      <c r="AD15">
+        <f>IF(OR('Private Interp'!AD15="",'Public Interp'!AD15=""),"",'Private Interp'!AD15+'Public Interp'!AD15)</f>
+        <v>0.44659736790218835</v>
+      </c>
+      <c r="AE15">
+        <f>IF(OR('Private Interp'!AE15="",'Public Interp'!AE15=""),"",'Private Interp'!AE15+'Public Interp'!AE15)</f>
+        <v>0.53842589274610153</v>
+      </c>
+      <c r="AF15">
+        <f>IF(OR('Private Interp'!AF15="",'Public Interp'!AF15=""),"",'Private Interp'!AF15+'Public Interp'!AF15)</f>
+        <v>3.3449999999999998</v>
+      </c>
+      <c r="AG15">
+        <f>IF(OR('Private Interp'!AG15="",'Public Interp'!AG15=""),"",'Private Interp'!AG15+'Public Interp'!AG15)</f>
+        <v>3.6399999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>2014</v>
+      </c>
+      <c r="B16">
+        <f>IF(OR('Private Interp'!B16="",'Public Interp'!B16=""),"",'Private Interp'!B16+'Public Interp'!B16)</f>
+        <v>2.742</v>
+      </c>
+      <c r="C16">
+        <f>IF(OR('Private Interp'!C16="",'Public Interp'!C16=""),"",'Private Interp'!C16+'Public Interp'!C16)</f>
+        <v>3.907</v>
+      </c>
+      <c r="D16">
+        <f>IF(OR('Private Interp'!D16="",'Public Interp'!D16=""),"",'Private Interp'!D16+'Public Interp'!D16)</f>
+        <v>2.2770000000000001</v>
+      </c>
+      <c r="E16">
+        <f>IF(OR('Private Interp'!E16="",'Public Interp'!E16=""),"",'Private Interp'!E16+'Public Interp'!E16)</f>
+        <v>3.1439999999999997</v>
+      </c>
+      <c r="F16">
+        <f>IF(OR('Private Interp'!F16="",'Public Interp'!F16=""),"",'Private Interp'!F16+'Public Interp'!F16)</f>
+        <v>2.6314874615176111</v>
+      </c>
+      <c r="G16" t="str">
+        <f>IF(OR('Private Interp'!G16="",'Public Interp'!G16=""),"",'Private Interp'!G16+'Public Interp'!G16)</f>
+        <v/>
+      </c>
+      <c r="H16">
+        <f>IF(OR('Private Interp'!H16="",'Public Interp'!H16=""),"",'Private Interp'!H16+'Public Interp'!H16)</f>
+        <v>0.11739780181361545</v>
+      </c>
+      <c r="I16">
+        <f>IF(OR('Private Interp'!I16="",'Public Interp'!I16=""),"",'Private Interp'!I16+'Public Interp'!I16)</f>
+        <v>-2.9799701981673699E-3</v>
+      </c>
+      <c r="J16">
+        <f>IF(OR('Private Interp'!J16="",'Public Interp'!J16=""),"",'Private Interp'!J16+'Public Interp'!J16)</f>
+        <v>-1.4009969735352956E-3</v>
+      </c>
+      <c r="K16">
+        <f>IF(OR('Private Interp'!K16="",'Public Interp'!K16=""),"",'Private Interp'!K16+'Public Interp'!K16)</f>
+        <v>-2.4722735525134043E-2</v>
+      </c>
+      <c r="L16">
+        <f>IF(OR('Private Interp'!L16="",'Public Interp'!L16=""),"",'Private Interp'!L16+'Public Interp'!L16)</f>
+        <v>4.8013515145267985E-2</v>
+      </c>
+      <c r="M16">
+        <f>IF(OR('Private Interp'!M16="",'Public Interp'!M16=""),"",'Private Interp'!M16+'Public Interp'!M16)</f>
+        <v>0.23826692888647213</v>
+      </c>
+      <c r="N16">
+        <f>IF(OR('Private Interp'!N16="",'Public Interp'!N16=""),"",'Private Interp'!N16+'Public Interp'!N16)</f>
+        <v>3.121</v>
+      </c>
+      <c r="O16">
+        <f>IF(OR('Private Interp'!O16="",'Public Interp'!O16=""),"",'Private Interp'!O16+'Public Interp'!O16)</f>
+        <v>3.032</v>
+      </c>
+      <c r="P16">
+        <f>IF(OR('Private Interp'!P16="",'Public Interp'!P16=""),"",'Private Interp'!P16+'Public Interp'!P16)</f>
+        <v>3.5879999999999996</v>
+      </c>
+      <c r="Q16">
+        <f>IF(OR('Private Interp'!Q16="",'Public Interp'!Q16=""),"",'Private Interp'!Q16+'Public Interp'!Q16)</f>
+        <v>2.569</v>
+      </c>
+      <c r="R16">
+        <f>IF(OR('Private Interp'!R16="",'Public Interp'!R16=""),"",'Private Interp'!R16+'Public Interp'!R16)</f>
+        <v>2.6059999999999999</v>
+      </c>
+      <c r="S16">
+        <f>IF(OR('Private Interp'!S16="",'Public Interp'!S16=""),"",'Private Interp'!S16+'Public Interp'!S16)</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T16">
+        <f>IF(OR('Private Interp'!T16="",'Public Interp'!T16=""),"",'Private Interp'!T16+'Public Interp'!T16)</f>
+        <v>1.8062816574325851</v>
+      </c>
+      <c r="U16" t="str">
+        <f>IF(OR('Private Interp'!U16="",'Public Interp'!U16=""),"",'Private Interp'!U16+'Public Interp'!U16)</f>
+        <v/>
+      </c>
+      <c r="V16" t="str">
+        <f>IF(OR('Private Interp'!V16="",'Public Interp'!V16=""),"",'Private Interp'!V16+'Public Interp'!V16)</f>
+        <v/>
+      </c>
+      <c r="W16">
+        <f>IF(OR('Private Interp'!W16="",'Public Interp'!W16=""),"",'Private Interp'!W16+'Public Interp'!W16)</f>
+        <v>-0.17516980988075015</v>
+      </c>
+      <c r="X16">
+        <f>IF(OR('Private Interp'!X16="",'Public Interp'!X16=""),"",'Private Interp'!X16+'Public Interp'!X16)</f>
+        <v>-1.8905549157440582E-2</v>
+      </c>
+      <c r="Y16">
+        <f>IF(OR('Private Interp'!Y16="",'Public Interp'!Y16=""),"",'Private Interp'!Y16+'Public Interp'!Y16)</f>
+        <v>0.1263925086144283</v>
+      </c>
+      <c r="Z16">
+        <f>IF(OR('Private Interp'!Z16="",'Public Interp'!Z16=""),"",'Private Interp'!Z16+'Public Interp'!Z16)</f>
+        <v>-5.8535904442045039E-2</v>
+      </c>
+      <c r="AA16">
+        <f>IF(OR('Private Interp'!AA16="",'Public Interp'!AA16=""),"",'Private Interp'!AA16+'Public Interp'!AA16)</f>
+        <v>-0.13005365441015415</v>
+      </c>
+      <c r="AB16">
+        <f>IF(OR('Private Interp'!AB16="",'Public Interp'!AB16=""),"",'Private Interp'!AB16+'Public Interp'!AB16)</f>
+        <v>-3.3098412736304983E-2</v>
+      </c>
+      <c r="AC16">
+        <f>IF(OR('Private Interp'!AC16="",'Public Interp'!AC16=""),"",'Private Interp'!AC16+'Public Interp'!AC16)</f>
+        <v>-5.0159243162991085E-2</v>
+      </c>
+      <c r="AD16">
+        <f>IF(OR('Private Interp'!AD16="",'Public Interp'!AD16=""),"",'Private Interp'!AD16+'Public Interp'!AD16)</f>
+        <v>0.44014176987959014</v>
+      </c>
+      <c r="AE16">
+        <f>IF(OR('Private Interp'!AE16="",'Public Interp'!AE16=""),"",'Private Interp'!AE16+'Public Interp'!AE16)</f>
+        <v>0.49355043568630252</v>
+      </c>
+      <c r="AF16">
+        <f>IF(OR('Private Interp'!AF16="",'Public Interp'!AF16=""),"",'Private Interp'!AF16+'Public Interp'!AF16)</f>
+        <v>3.7770000000000001</v>
+      </c>
+      <c r="AG16">
+        <f>IF(OR('Private Interp'!AG16="",'Public Interp'!AG16=""),"",'Private Interp'!AG16+'Public Interp'!AG16)</f>
+        <v>3.7040000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>2015</v>
+      </c>
+      <c r="B17">
+        <f>IF(OR('Private Interp'!B17="",'Public Interp'!B17=""),"",'Private Interp'!B17+'Public Interp'!B17)</f>
+        <v>2.86</v>
+      </c>
+      <c r="C17">
+        <f>IF(OR('Private Interp'!C17="",'Public Interp'!C17=""),"",'Private Interp'!C17+'Public Interp'!C17)</f>
+        <v>3.8810000000000002</v>
+      </c>
+      <c r="D17">
+        <f>IF(OR('Private Interp'!D17="",'Public Interp'!D17=""),"",'Private Interp'!D17+'Public Interp'!D17)</f>
+        <v>2.2050000000000001</v>
+      </c>
+      <c r="E17">
+        <f>IF(OR('Private Interp'!E17="",'Public Interp'!E17=""),"",'Private Interp'!E17+'Public Interp'!E17)</f>
+        <v>3.2409999999999997</v>
+      </c>
+      <c r="F17">
+        <f>IF(OR('Private Interp'!F17="",'Public Interp'!F17=""),"",'Private Interp'!F17+'Public Interp'!F17)</f>
+        <v>2.6799769446061852</v>
+      </c>
+      <c r="G17" t="str">
+        <f>IF(OR('Private Interp'!G17="",'Public Interp'!G17=""),"",'Private Interp'!G17+'Public Interp'!G17)</f>
+        <v/>
+      </c>
+      <c r="H17">
+        <f>IF(OR('Private Interp'!H17="",'Public Interp'!H17=""),"",'Private Interp'!H17+'Public Interp'!H17)</f>
+        <v>8.3966680240075087E-2</v>
+      </c>
+      <c r="I17">
+        <f>IF(OR('Private Interp'!I17="",'Public Interp'!I17=""),"",'Private Interp'!I17+'Public Interp'!I17)</f>
+        <v>-2.3027998200789879E-2</v>
+      </c>
+      <c r="J17">
+        <f>IF(OR('Private Interp'!J17="",'Public Interp'!J17=""),"",'Private Interp'!J17+'Public Interp'!J17)</f>
+        <v>-6.3719491621130733E-2</v>
+      </c>
+      <c r="K17">
+        <f>IF(OR('Private Interp'!K17="",'Public Interp'!K17=""),"",'Private Interp'!K17+'Public Interp'!K17)</f>
+        <v>0.43703127840925826</v>
+      </c>
+      <c r="L17">
+        <f>IF(OR('Private Interp'!L17="",'Public Interp'!L17=""),"",'Private Interp'!L17+'Public Interp'!L17)</f>
+        <v>0.10972617474720403</v>
+      </c>
+      <c r="M17">
+        <f>IF(OR('Private Interp'!M17="",'Public Interp'!M17=""),"",'Private Interp'!M17+'Public Interp'!M17)</f>
+        <v>0.26588407462051511</v>
+      </c>
+      <c r="N17">
+        <f>IF(OR('Private Interp'!N17="",'Public Interp'!N17=""),"",'Private Interp'!N17+'Public Interp'!N17)</f>
+        <v>3.0605481003447319</v>
+      </c>
+      <c r="O17">
+        <f>IF(OR('Private Interp'!O17="",'Public Interp'!O17=""),"",'Private Interp'!O17+'Public Interp'!O17)</f>
+        <v>2.9696294036063207</v>
+      </c>
+      <c r="P17">
+        <f>IF(OR('Private Interp'!P17="",'Public Interp'!P17=""),"",'Private Interp'!P17+'Public Interp'!P17)</f>
+        <v>3.4060000000000001</v>
+      </c>
+      <c r="Q17">
+        <f>IF(OR('Private Interp'!Q17="",'Public Interp'!Q17=""),"",'Private Interp'!Q17+'Public Interp'!Q17)</f>
+        <v>2.5259999999999998</v>
+      </c>
+      <c r="R17">
+        <f>IF(OR('Private Interp'!R17="",'Public Interp'!R17=""),"",'Private Interp'!R17+'Public Interp'!R17)</f>
+        <v>2.5649999999999999</v>
+      </c>
+      <c r="S17">
+        <f>IF(OR('Private Interp'!S17="",'Public Interp'!S17=""),"",'Private Interp'!S17+'Public Interp'!S17)</f>
+        <v>2.2119999999999997</v>
+      </c>
+      <c r="T17">
+        <f>IF(OR('Private Interp'!T17="",'Public Interp'!T17=""),"",'Private Interp'!T17+'Public Interp'!T17)</f>
+        <v>1.8073180083814706</v>
+      </c>
+      <c r="U17" t="str">
+        <f>IF(OR('Private Interp'!U17="",'Public Interp'!U17=""),"",'Private Interp'!U17+'Public Interp'!U17)</f>
+        <v/>
+      </c>
+      <c r="V17" t="str">
+        <f>IF(OR('Private Interp'!V17="",'Public Interp'!V17=""),"",'Private Interp'!V17+'Public Interp'!V17)</f>
+        <v/>
+      </c>
+      <c r="W17" t="str">
+        <f>IF(OR('Private Interp'!W17="",'Public Interp'!W17=""),"",'Private Interp'!W17+'Public Interp'!W17)</f>
+        <v/>
+      </c>
+      <c r="X17" t="str">
+        <f>IF(OR('Private Interp'!X17="",'Public Interp'!X17=""),"",'Private Interp'!X17+'Public Interp'!X17)</f>
+        <v/>
+      </c>
+      <c r="Y17">
+        <f>IF(OR('Private Interp'!Y17="",'Public Interp'!Y17=""),"",'Private Interp'!Y17+'Public Interp'!Y17)</f>
+        <v>-0.10597520295429286</v>
+      </c>
+      <c r="Z17">
+        <f>IF(OR('Private Interp'!Z17="",'Public Interp'!Z17=""),"",'Private Interp'!Z17+'Public Interp'!Z17)</f>
+        <v>-2.3965042392545932E-2</v>
+      </c>
+      <c r="AA17">
+        <f>IF(OR('Private Interp'!AA17="",'Public Interp'!AA17=""),"",'Private Interp'!AA17+'Public Interp'!AA17)</f>
+        <v>-8.7194652320792987E-2</v>
+      </c>
+      <c r="AB17">
+        <f>IF(OR('Private Interp'!AB17="",'Public Interp'!AB17=""),"",'Private Interp'!AB17+'Public Interp'!AB17)</f>
+        <v>5.6769306344800596E-2</v>
+      </c>
+      <c r="AC17">
+        <f>IF(OR('Private Interp'!AC17="",'Public Interp'!AC17=""),"",'Private Interp'!AC17+'Public Interp'!AC17)</f>
+        <v>6.1395452020784795E-3</v>
+      </c>
+      <c r="AD17">
+        <f>IF(OR('Private Interp'!AD17="",'Public Interp'!AD17=""),"",'Private Interp'!AD17+'Public Interp'!AD17)</f>
+        <v>0.39743858880106103</v>
+      </c>
+      <c r="AE17">
+        <f>IF(OR('Private Interp'!AE17="",'Public Interp'!AE17=""),"",'Private Interp'!AE17+'Public Interp'!AE17)</f>
+        <v>0.49029179398469896</v>
+      </c>
+      <c r="AF17">
+        <f>IF(OR('Private Interp'!AF17="",'Public Interp'!AF17=""),"",'Private Interp'!AF17+'Public Interp'!AF17)</f>
+        <v>3.8449999999999998</v>
+      </c>
+      <c r="AG17">
+        <f>IF(OR('Private Interp'!AG17="",'Public Interp'!AG17=""),"",'Private Interp'!AG17+'Public Interp'!AG17)</f>
+        <v>3.6080000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E769F5-59CA-4795-8B33-0EF0F059F992}">
+  <dimension ref="A1:AI23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="7" max="12" width="0" hidden="1" customWidth="1"/>
+    <col min="22" max="30" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>2000</v>
+      </c>
+      <c r="B2">
+        <v>2.4</v>
+      </c>
+      <c r="R2">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <f t="shared" ref="A4:A9" si="0">A3+1</f>
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>2005</v>
+      </c>
+      <c r="B7">
+        <v>2.5</v>
+      </c>
+      <c r="R7">
+        <v>2.5</v>
+      </c>
+      <c r="AH7">
+        <v>2.7</v>
+      </c>
+      <c r="AI7">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>2008</v>
+      </c>
+      <c r="B10">
+        <v>2.4</v>
+      </c>
+      <c r="R10">
+        <v>2.6</v>
+      </c>
+      <c r="AH10">
+        <v>2.8</v>
+      </c>
+      <c r="AI10">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>2009</v>
+      </c>
+      <c r="B11">
+        <v>2.6</v>
+      </c>
+      <c r="R11">
+        <v>2.8</v>
+      </c>
+      <c r="AH11">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>2010</v>
+      </c>
+      <c r="B12">
+        <v>2.7</v>
+      </c>
+      <c r="R12">
+        <v>2.9</v>
+      </c>
+      <c r="AH12">
+        <v>2.9</v>
+      </c>
+      <c r="AI12">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>2011</v>
+      </c>
+      <c r="B13">
+        <v>2.6</v>
+      </c>
+      <c r="C13">
+        <v>3.9</v>
+      </c>
+      <c r="R13">
+        <v>2.9</v>
+      </c>
+      <c r="AG13">
+        <v>3.8</v>
+      </c>
+      <c r="AH13">
+        <v>2.8</v>
+      </c>
+      <c r="AI13">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>2012</v>
+      </c>
+      <c r="B14">
+        <v>2.5</v>
+      </c>
+      <c r="C14">
+        <v>3.9</v>
+      </c>
+      <c r="D14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E14">
+        <v>3.1</v>
+      </c>
+      <c r="F14">
+        <v>2.6</v>
+      </c>
+      <c r="N14">
+        <v>3.2</v>
+      </c>
+      <c r="O14">
+        <f>O15+AD14</f>
+        <v>2.8857142857142857</v>
+      </c>
+      <c r="P14">
+        <v>3.4</v>
+      </c>
+      <c r="Q14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R14">
+        <v>2.9</v>
+      </c>
+      <c r="S14">
+        <v>2.9</v>
+      </c>
+      <c r="T14">
+        <v>2.1</v>
+      </c>
+      <c r="U14">
+        <v>2.9</v>
+      </c>
+      <c r="W14">
+        <f>N14-N15</f>
+        <v>-9.9999999999999645E-2</v>
+      </c>
+      <c r="X14">
+        <f t="shared" ref="X14:AC14" si="1">P14-P15</f>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="1"/>
+        <v>-0.10000000000000009</v>
+      </c>
+      <c r="AC14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <f>AVERAGE(W14:AC14)</f>
+        <v>-1.4285714285714235E-2</v>
+      </c>
+      <c r="AF14">
+        <v>3.2</v>
+      </c>
+      <c r="AG14">
+        <v>3.8</v>
+      </c>
+      <c r="AH14">
+        <v>2.7</v>
+      </c>
+      <c r="AI14">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>2013</v>
+      </c>
+      <c r="B15">
+        <v>2.6</v>
+      </c>
+      <c r="C15">
+        <v>3.9</v>
+      </c>
+      <c r="D15">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E15">
+        <v>3.2</v>
+      </c>
+      <c r="F15">
+        <f>F14+L15</f>
+        <v>2.6500000000000004</v>
+      </c>
+      <c r="H15">
+        <f>B15-B14</f>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="I15">
+        <f>C15-C14</f>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f>D15-D14</f>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f>E15-E14</f>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="L15">
+        <f>AVERAGE(H15:K15)</f>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="N15">
+        <v>3.3</v>
+      </c>
+      <c r="O15">
+        <v>2.9</v>
+      </c>
+      <c r="P15">
+        <v>3.3</v>
+      </c>
+      <c r="Q15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R15">
+        <v>2.9</v>
+      </c>
+      <c r="S15">
+        <v>2.9</v>
+      </c>
+      <c r="T15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="U15">
+        <v>2.9</v>
+      </c>
+      <c r="AF15">
+        <v>3.4</v>
+      </c>
+      <c r="AG15">
+        <v>3.6</v>
+      </c>
+      <c r="AH15">
+        <v>2.8</v>
+      </c>
+      <c r="AI15">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>2014</v>
+      </c>
+      <c r="B16">
+        <v>2.7</v>
+      </c>
+      <c r="C16">
+        <v>3.9</v>
+      </c>
+      <c r="D16">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E16">
+        <v>3.1</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ref="F16:F17" si="2">F15+L16</f>
+        <v>2.6500000000000004</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ref="H16:K17" si="3">B16-B15</f>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="3"/>
+        <v>-0.10000000000000009</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ref="L16:L17" si="4">AVERAGE(H16:K16)</f>
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>3.3</v>
+      </c>
+      <c r="O16">
+        <v>3.1</v>
+      </c>
+      <c r="P16">
+        <v>3.3</v>
+      </c>
+      <c r="Q16">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R16">
+        <v>2.9</v>
+      </c>
+      <c r="S16">
+        <v>2.7</v>
+      </c>
+      <c r="T16">
+        <v>2.1</v>
+      </c>
+      <c r="U16">
+        <v>2.8</v>
+      </c>
+      <c r="AF16">
+        <v>3.4</v>
+      </c>
+      <c r="AG16">
+        <v>3.6</v>
+      </c>
+      <c r="AH16">
+        <v>2.8</v>
+      </c>
+      <c r="AI16">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>2015</v>
+      </c>
+      <c r="B17">
+        <v>2.9</v>
+      </c>
+      <c r="C17">
+        <v>3.9</v>
+      </c>
+      <c r="D17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E17">
+        <v>3.2</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>2.7</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="3"/>
+        <v>0.19999999999999973</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>-9.9999999999999645E-2</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="3"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="4"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="N17">
+        <v>3.3</v>
+      </c>
+      <c r="O17">
+        <f>O16+AD17</f>
+        <v>3.0428571428571431</v>
+      </c>
+      <c r="P17">
+        <v>3.2</v>
+      </c>
+      <c r="Q17">
+        <v>2.1</v>
+      </c>
+      <c r="R17">
+        <v>2.9</v>
+      </c>
+      <c r="S17">
+        <v>2.5</v>
+      </c>
+      <c r="T17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="U17">
+        <v>2.7</v>
+      </c>
+      <c r="W17">
+        <f>N17-N16</f>
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <f t="shared" ref="X17:AC17" si="5">P17-P16</f>
+        <v>-9.9999999999999645E-2</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="5"/>
+        <v>-0.10000000000000009</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" si="5"/>
+        <v>-0.20000000000000018</v>
+      </c>
+      <c r="AB17">
+        <f t="shared" si="5"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="AC17">
+        <f t="shared" si="5"/>
+        <v>-9.9999999999999645E-2</v>
+      </c>
+      <c r="AD17">
+        <f>AVERAGE(W17:AC17)</f>
+        <v>-5.7142857142857065E-2</v>
+      </c>
+      <c r="AF17">
+        <v>3.3</v>
+      </c>
+      <c r="AG17">
+        <v>3.6</v>
+      </c>
+      <c r="AH17">
+        <v>2.7</v>
+      </c>
+      <c r="AI17">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>